<commit_message>
Navigation map into client
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D00BEC-8E29-46B4-A4CF-8605736E670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C86A76A-1D29-4D6A-B07C-26D7F0050026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1331,91 +1331,91 @@
                   <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3034,21 +3034,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="H21" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" customWidth="1"/>
-    <col min="39" max="40" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="39" max="40" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:69" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:69" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
@@ -3120,7 +3120,7 @@
       <c r="BP2" s="34"/>
       <c r="BQ2" s="1"/>
     </row>
-    <row r="3" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
       <c r="D3" s="45"/>
@@ -3189,7 +3189,7 @@
       <c r="BO3" s="3"/>
       <c r="BP3" s="3"/>
     </row>
-    <row r="4" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="27" t="s">
@@ -3592,7 +3592,7 @@
       </c>
       <c r="BQ5" s="1"/>
     </row>
-    <row r="6" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B6" s="31">
         <v>1</v>
       </c>
@@ -3669,7 +3669,7 @@
       <c r="BO6" s="2"/>
       <c r="BP6" s="2"/>
     </row>
-    <row r="7" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B7" s="31">
         <v>2</v>
       </c>
@@ -3746,7 +3746,7 @@
       <c r="BO7" s="2"/>
       <c r="BP7" s="2"/>
     </row>
-    <row r="8" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B8" s="31">
         <v>3</v>
       </c>
@@ -3823,7 +3823,7 @@
       <c r="BO8" s="2"/>
       <c r="BP8" s="2"/>
     </row>
-    <row r="9" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B9" s="31">
         <v>4</v>
       </c>
@@ -3900,7 +3900,7 @@
       <c r="BO9" s="2"/>
       <c r="BP9" s="2"/>
     </row>
-    <row r="10" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B10" s="31">
         <v>5</v>
       </c>
@@ -3975,7 +3975,7 @@
       <c r="BO10" s="2"/>
       <c r="BP10" s="2"/>
     </row>
-    <row r="11" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B11" s="31">
         <v>6</v>
       </c>
@@ -4052,7 +4052,7 @@
       <c r="BO11" s="2"/>
       <c r="BP11" s="2"/>
     </row>
-    <row r="12" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B12" s="31">
         <v>7</v>
       </c>
@@ -4129,7 +4129,7 @@
       <c r="BO12" s="2"/>
       <c r="BP12" s="2"/>
     </row>
-    <row r="13" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B13" s="31">
         <v>8</v>
       </c>
@@ -4204,7 +4204,7 @@
       <c r="BO13" s="2"/>
       <c r="BP13" s="2"/>
     </row>
-    <row r="14" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B14" s="31">
         <v>9</v>
       </c>
@@ -4279,7 +4279,7 @@
       <c r="BO14" s="2"/>
       <c r="BP14" s="2"/>
     </row>
-    <row r="15" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B15" s="31">
         <v>10</v>
       </c>
@@ -4354,7 +4354,7 @@
       <c r="BO15" s="2"/>
       <c r="BP15" s="2"/>
     </row>
-    <row r="16" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B16" s="31">
         <v>11</v>
       </c>
@@ -4429,14 +4429,14 @@
       <c r="BO16" s="2"/>
       <c r="BP16" s="2"/>
     </row>
-    <row r="17" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B17" s="31">
         <v>12</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="15">
         <v>2</v>
       </c>
       <c r="E17" s="17"/>
@@ -4467,20 +4467,22 @@
       <c r="Z17" s="17">
         <v>1</v>
       </c>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2"/>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
-      <c r="AL17" s="2"/>
-      <c r="AM17" s="2"/>
-      <c r="AN17" s="2"/>
+      <c r="AA17" s="21"/>
+      <c r="AB17" s="21"/>
+      <c r="AC17" s="21"/>
+      <c r="AD17" s="21"/>
+      <c r="AE17" s="21"/>
+      <c r="AF17" s="21"/>
+      <c r="AG17" s="21"/>
+      <c r="AH17" s="21"/>
+      <c r="AI17" s="21"/>
+      <c r="AJ17" s="21"/>
+      <c r="AK17" s="21"/>
+      <c r="AL17" s="21"/>
+      <c r="AM17" s="21"/>
+      <c r="AN17" s="15">
+        <v>1</v>
+      </c>
       <c r="AO17" s="2"/>
       <c r="AP17" s="2"/>
       <c r="AQ17" s="2"/>
@@ -4510,7 +4512,7 @@
       <c r="BO17" s="2"/>
       <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B18" s="31">
         <v>13</v>
       </c>
@@ -4585,7 +4587,7 @@
       <c r="BO18" s="2"/>
       <c r="BP18" s="2"/>
     </row>
-    <row r="19" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B19" s="31">
         <v>14</v>
       </c>
@@ -4662,7 +4664,7 @@
       <c r="BO19" s="2"/>
       <c r="BP19" s="2"/>
     </row>
-    <row r="20" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B20" s="31">
         <v>15</v>
       </c>
@@ -4737,7 +4739,7 @@
       <c r="BO20" s="2"/>
       <c r="BP20" s="2"/>
     </row>
-    <row r="21" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B21" s="31">
         <v>16</v>
       </c>
@@ -4812,7 +4814,7 @@
       <c r="BO21" s="2"/>
       <c r="BP21" s="2"/>
     </row>
-    <row r="22" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B22" s="31">
         <v>17</v>
       </c>
@@ -4887,7 +4889,7 @@
       <c r="BO22" s="2"/>
       <c r="BP22" s="2"/>
     </row>
-    <row r="23" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B23" s="31">
         <v>18</v>
       </c>
@@ -4962,7 +4964,7 @@
       <c r="BO23" s="2"/>
       <c r="BP23" s="2"/>
     </row>
-    <row r="24" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B24" s="31">
         <v>19</v>
       </c>
@@ -5037,7 +5039,7 @@
       <c r="BO24" s="2"/>
       <c r="BP24" s="2"/>
     </row>
-    <row r="25" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B25" s="31">
         <v>20</v>
       </c>
@@ -5116,7 +5118,7 @@
       <c r="BO25" s="2"/>
       <c r="BP25" s="2"/>
     </row>
-    <row r="26" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B26" s="31">
         <v>21</v>
       </c>
@@ -5191,7 +5193,7 @@
       <c r="BO26" s="2"/>
       <c r="BP26" s="2"/>
     </row>
-    <row r="27" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B27" s="31">
         <v>22</v>
       </c>
@@ -5266,7 +5268,7 @@
       <c r="BO27" s="2"/>
       <c r="BP27" s="2"/>
     </row>
-    <row r="28" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B28" s="31">
         <v>23</v>
       </c>
@@ -5341,7 +5343,7 @@
       <c r="BO28" s="2"/>
       <c r="BP28" s="2"/>
     </row>
-    <row r="29" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B29" s="31">
         <v>24</v>
       </c>
@@ -5416,7 +5418,7 @@
       <c r="BO29" s="2"/>
       <c r="BP29" s="2"/>
     </row>
-    <row r="30" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B30" s="31">
         <v>25</v>
       </c>
@@ -5491,7 +5493,7 @@
       <c r="BO30" s="2"/>
       <c r="BP30" s="2"/>
     </row>
-    <row r="31" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B31" s="31">
         <v>26</v>
       </c>
@@ -5566,7 +5568,7 @@
       <c r="BO31" s="2"/>
       <c r="BP31" s="2"/>
     </row>
-    <row r="32" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B32" s="31">
         <v>27</v>
       </c>
@@ -5641,7 +5643,7 @@
       <c r="BO32" s="2"/>
       <c r="BP32" s="2"/>
     </row>
-    <row r="33" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B33" s="31">
         <v>28</v>
       </c>
@@ -5716,7 +5718,7 @@
       <c r="BO33" s="2"/>
       <c r="BP33" s="2"/>
     </row>
-    <row r="34" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B34" s="31">
         <v>29</v>
       </c>
@@ -5791,7 +5793,7 @@
       <c r="BO34" s="2"/>
       <c r="BP34" s="2"/>
     </row>
-    <row r="35" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B35" s="31">
         <v>30</v>
       </c>
@@ -5866,7 +5868,7 @@
       <c r="BO35" s="2"/>
       <c r="BP35" s="2"/>
     </row>
-    <row r="36" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B36" s="31">
         <v>31</v>
       </c>
@@ -5941,7 +5943,7 @@
       <c r="BO36" s="2"/>
       <c r="BP36" s="2"/>
     </row>
-    <row r="37" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B37" s="32">
         <v>32</v>
       </c>
@@ -6016,7 +6018,7 @@
       <c r="BO37" s="4"/>
       <c r="BP37" s="4"/>
     </row>
-    <row r="38" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B38" s="33">
         <v>33</v>
       </c>
@@ -6093,7 +6095,7 @@
       <c r="BO38" s="4"/>
       <c r="BP38" s="4"/>
     </row>
-    <row r="39" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B39" s="32">
         <v>34</v>
       </c>
@@ -6170,7 +6172,7 @@
       <c r="BO39" s="2"/>
       <c r="BP39" s="2"/>
     </row>
-    <row r="40" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B40" s="33">
         <v>35</v>
       </c>
@@ -6247,7 +6249,7 @@
       <c r="BO40" s="2"/>
       <c r="BP40" s="2"/>
     </row>
-    <row r="41" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B41" s="32">
         <v>36</v>
       </c>
@@ -6324,7 +6326,7 @@
       <c r="BO41" s="2"/>
       <c r="BP41" s="2"/>
     </row>
-    <row r="42" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B42" s="33">
         <v>37</v>
       </c>
@@ -6401,7 +6403,7 @@
       <c r="BO42" s="2"/>
       <c r="BP42" s="2"/>
     </row>
-    <row r="43" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B43" s="32">
         <v>38</v>
       </c>
@@ -6476,7 +6478,7 @@
       <c r="BO43" s="2"/>
       <c r="BP43" s="2"/>
     </row>
-    <row r="44" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B44" s="33">
         <v>39</v>
       </c>
@@ -6553,7 +6555,7 @@
       <c r="BO44" s="2"/>
       <c r="BP44" s="2"/>
     </row>
-    <row r="45" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B45" s="32">
         <v>40</v>
       </c>
@@ -6626,7 +6628,7 @@
       <c r="BO45" s="2"/>
       <c r="BP45" s="2"/>
     </row>
-    <row r="46" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B46" s="33">
         <v>41</v>
       </c>
@@ -6699,7 +6701,7 @@
       <c r="BO46" s="2"/>
       <c r="BP46" s="2"/>
     </row>
-    <row r="47" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B47" s="23"/>
       <c r="C47" s="23"/>
       <c r="D47" s="24"/>
@@ -6768,7 +6770,7 @@
       <c r="BO47" s="2"/>
       <c r="BP47" s="2"/>
     </row>
-    <row r="48" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
       <c r="D48" s="26"/>
@@ -6837,7 +6839,7 @@
       <c r="BO48" s="4"/>
       <c r="BP48" s="4"/>
     </row>
-    <row r="49" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B49" s="38" t="s">
         <v>69</v>
       </c>
@@ -6988,122 +6990,122 @@
       </c>
       <c r="AN49" s="5">
         <f t="shared" ref="AN49" si="24">AM49-SUM(AN6:AN48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AO49" s="5">
         <f t="shared" ref="AO49" si="25">AN49-SUM(AO6:AO48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AP49" s="5">
         <f t="shared" ref="AP49" si="26">AO49-SUM(AP6:AP48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AQ49" s="5">
         <f t="shared" ref="AQ49" si="27">AP49-SUM(AQ6:AQ48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AR49" s="5">
         <f t="shared" ref="AR49" si="28">AQ49-SUM(AR6:AR48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AS49" s="5">
         <f t="shared" ref="AS49" si="29">AR49-SUM(AS6:AS48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AT49" s="5">
         <f t="shared" ref="AT49" si="30">AS49-SUM(AT6:AT48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AU49" s="5">
         <f t="shared" ref="AU49" si="31">AT49-SUM(AU6:AU48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AV49" s="5">
         <f t="shared" ref="AV49" si="32">AU49-SUM(AV6:AV48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AW49" s="5">
         <f t="shared" ref="AW49" si="33">AV49-SUM(AW6:AW48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX49" s="5">
         <f t="shared" ref="AX49" si="34">AW49-SUM(AX6:AX48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AY49" s="5">
         <f t="shared" ref="AY49" si="35">AX49-SUM(AY6:AY48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AZ49" s="5">
         <f>AY49-SUM(AZ6:AZ48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BA49" s="5">
         <f t="shared" ref="BA49" si="36">AZ49-SUM(BA6:BA48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BB49" s="5">
         <f t="shared" ref="BB49" si="37">BA49-SUM(BB6:BB48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC49" s="5">
         <f t="shared" ref="BC49" si="38">BB49-SUM(BC6:BC48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BD49" s="5">
         <f t="shared" ref="BD49" si="39">BC49-SUM(BD6:BD48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BE49" s="5">
         <f t="shared" ref="BE49" si="40">BD49-SUM(BE6:BE48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BF49" s="5">
         <f t="shared" ref="BF49" si="41">BE49-SUM(BF6:BF48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BG49" s="5">
         <f t="shared" ref="BG49" si="42">BF49-SUM(BG6:BG48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BH49" s="5">
         <f t="shared" ref="BH49" si="43">BG49-SUM(BH6:BH48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BI49" s="5">
         <f t="shared" ref="BI49" si="44">BH49-SUM(BI6:BI48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BJ49" s="5">
         <f t="shared" ref="BJ49" si="45">BI49-SUM(BJ6:BJ48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BK49" s="5">
         <f t="shared" ref="BK49" si="46">BJ49-SUM(BK6:BK48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BL49" s="5">
         <f t="shared" ref="BL49" si="47">BK49-SUM(BL6:BL48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BM49" s="5">
         <f t="shared" ref="BM49" si="48">BL49-SUM(BM6:BM48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BN49" s="5">
         <f t="shared" ref="BN49" si="49">BM49-SUM(BN6:BN48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BO49" s="5">
         <f>BN49-SUM(BO6:BO48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BP49" s="13">
         <f t="shared" ref="BP49" si="50">BO49-SUM(BP6:BP48)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="50" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="36" t="s">
         <v>70</v>
       </c>
@@ -7369,17 +7371,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B51" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B52" s="19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="20" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
Herberg create, update, delete klaar.
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AA1D44-2233-4FF2-8426-B5FA16E55204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD9EC80-81D3-4CC3-AC7D-9DB8F99F4580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
@@ -752,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -774,9 +774,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,9 +830,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1340,82 +1334,82 @@
                   <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>46.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>44.5</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3035,7 +3029,7 @@
   <dimension ref="B1:BQ53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3049,98 +3043,98 @@
   <sheetData>
     <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:69" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
-      <c r="AW2" s="34"/>
-      <c r="AX2" s="34"/>
-      <c r="AY2" s="34"/>
-      <c r="AZ2" s="34"/>
-      <c r="BA2" s="34"/>
-      <c r="BB2" s="34"/>
-      <c r="BC2" s="34"/>
-      <c r="BD2" s="34"/>
-      <c r="BE2" s="34"/>
-      <c r="BF2" s="34"/>
-      <c r="BG2" s="34"/>
-      <c r="BH2" s="34"/>
-      <c r="BI2" s="34"/>
-      <c r="BJ2" s="34"/>
-      <c r="BK2" s="34"/>
-      <c r="BL2" s="34"/>
-      <c r="BM2" s="34"/>
-      <c r="BN2" s="34"/>
-      <c r="BO2" s="34"/>
-      <c r="BP2" s="34"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="32"/>
+      <c r="BH2" s="32"/>
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="32"/>
+      <c r="BK2" s="32"/>
+      <c r="BL2" s="32"/>
+      <c r="BM2" s="32"/>
+      <c r="BN2" s="32"/>
+      <c r="BO2" s="32"/>
+      <c r="BP2" s="32"/>
       <c r="BQ2" s="1"/>
     </row>
     <row r="3" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -3190,419 +3184,419 @@
       <c r="BP3" s="3"/>
     </row>
     <row r="4" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>45166</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <v>45167</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G4" s="27">
         <v>45168</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="27">
         <v>45169</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="27">
         <v>45170</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="27">
         <v>45171</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="27">
         <v>45172</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="27">
         <v>45173</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="27">
         <v>45174</v>
       </c>
-      <c r="N4" s="28">
+      <c r="N4" s="27">
         <v>45175</v>
       </c>
-      <c r="O4" s="28">
+      <c r="O4" s="27">
         <v>45176</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="27">
         <v>45177</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="Q4" s="27">
         <v>45178</v>
       </c>
-      <c r="R4" s="28">
+      <c r="R4" s="27">
         <v>45179</v>
       </c>
-      <c r="S4" s="28">
+      <c r="S4" s="27">
         <v>45180</v>
       </c>
-      <c r="T4" s="28">
+      <c r="T4" s="27">
         <v>45181</v>
       </c>
-      <c r="U4" s="28">
+      <c r="U4" s="27">
         <v>45182</v>
       </c>
-      <c r="V4" s="28">
+      <c r="V4" s="27">
         <v>45183</v>
       </c>
-      <c r="W4" s="28">
+      <c r="W4" s="27">
         <v>45184</v>
       </c>
-      <c r="X4" s="28">
+      <c r="X4" s="27">
         <v>45185</v>
       </c>
-      <c r="Y4" s="28">
+      <c r="Y4" s="27">
         <v>45186</v>
       </c>
-      <c r="Z4" s="28">
+      <c r="Z4" s="27">
         <v>45187</v>
       </c>
-      <c r="AA4" s="28">
+      <c r="AA4" s="27">
         <v>45188</v>
       </c>
-      <c r="AB4" s="28">
+      <c r="AB4" s="27">
         <v>45189</v>
       </c>
-      <c r="AC4" s="28">
+      <c r="AC4" s="27">
         <v>45190</v>
       </c>
-      <c r="AD4" s="28">
+      <c r="AD4" s="27">
         <v>45191</v>
       </c>
-      <c r="AE4" s="28">
+      <c r="AE4" s="27">
         <v>45192</v>
       </c>
-      <c r="AF4" s="28">
+      <c r="AF4" s="27">
         <v>45193</v>
       </c>
-      <c r="AG4" s="28">
+      <c r="AG4" s="27">
         <v>45194</v>
       </c>
-      <c r="AH4" s="28">
+      <c r="AH4" s="27">
         <v>45195</v>
       </c>
-      <c r="AI4" s="28">
+      <c r="AI4" s="27">
         <v>45196</v>
       </c>
-      <c r="AJ4" s="28">
+      <c r="AJ4" s="27">
         <v>45197</v>
       </c>
-      <c r="AK4" s="28">
+      <c r="AK4" s="27">
         <v>45198</v>
       </c>
-      <c r="AL4" s="28">
+      <c r="AL4" s="27">
         <v>45199</v>
       </c>
-      <c r="AM4" s="28">
+      <c r="AM4" s="27">
         <v>45200</v>
       </c>
-      <c r="AN4" s="28">
+      <c r="AN4" s="27">
         <v>45201</v>
       </c>
-      <c r="AO4" s="28">
+      <c r="AO4" s="27">
         <v>45202</v>
       </c>
-      <c r="AP4" s="28">
+      <c r="AP4" s="27">
         <v>45203</v>
       </c>
-      <c r="AQ4" s="28">
+      <c r="AQ4" s="27">
         <v>45204</v>
       </c>
-      <c r="AR4" s="28">
+      <c r="AR4" s="27">
         <v>45205</v>
       </c>
-      <c r="AS4" s="28">
+      <c r="AS4" s="27">
         <v>45206</v>
       </c>
-      <c r="AT4" s="28">
+      <c r="AT4" s="27">
         <v>45207</v>
       </c>
-      <c r="AU4" s="28">
+      <c r="AU4" s="27">
         <v>45208</v>
       </c>
-      <c r="AV4" s="28">
+      <c r="AV4" s="27">
         <v>45209</v>
       </c>
-      <c r="AW4" s="28">
+      <c r="AW4" s="27">
         <v>45210</v>
       </c>
-      <c r="AX4" s="28">
+      <c r="AX4" s="27">
         <v>45211</v>
       </c>
-      <c r="AY4" s="28">
+      <c r="AY4" s="27">
         <v>45212</v>
       </c>
-      <c r="AZ4" s="28">
+      <c r="AZ4" s="27">
         <v>45213</v>
       </c>
-      <c r="BA4" s="28">
+      <c r="BA4" s="27">
         <v>45214</v>
       </c>
-      <c r="BB4" s="28">
+      <c r="BB4" s="27">
         <v>45215</v>
       </c>
-      <c r="BC4" s="28">
+      <c r="BC4" s="27">
         <v>45216</v>
       </c>
-      <c r="BD4" s="28">
+      <c r="BD4" s="27">
         <v>45217</v>
       </c>
-      <c r="BE4" s="28">
+      <c r="BE4" s="27">
         <v>45218</v>
       </c>
-      <c r="BF4" s="28">
+      <c r="BF4" s="27">
         <v>45219</v>
       </c>
-      <c r="BG4" s="28">
+      <c r="BG4" s="27">
         <v>45220</v>
       </c>
-      <c r="BH4" s="28">
+      <c r="BH4" s="27">
         <v>45221</v>
       </c>
-      <c r="BI4" s="28">
+      <c r="BI4" s="27">
         <v>45222</v>
       </c>
-      <c r="BJ4" s="28">
+      <c r="BJ4" s="27">
         <v>45223</v>
       </c>
-      <c r="BK4" s="28">
+      <c r="BK4" s="27">
         <v>45224</v>
       </c>
-      <c r="BL4" s="28">
+      <c r="BL4" s="27">
         <v>45225</v>
       </c>
-      <c r="BM4" s="28">
+      <c r="BM4" s="27">
         <v>45226</v>
       </c>
-      <c r="BN4" s="28">
+      <c r="BN4" s="27">
         <v>45227</v>
       </c>
-      <c r="BO4" s="28">
+      <c r="BO4" s="27">
         <v>45228</v>
       </c>
-      <c r="BP4" s="28">
+      <c r="BP4" s="27">
         <v>45229</v>
       </c>
     </row>
     <row r="5" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="27" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="27" t="s">
+      <c r="N5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="27" t="s">
+      <c r="O5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="27" t="s">
+      <c r="P5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="27" t="s">
+      <c r="Q5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="27" t="s">
+      <c r="R5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="27" t="s">
+      <c r="S5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="27" t="s">
+      <c r="T5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="U5" s="27" t="s">
+      <c r="U5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="27" t="s">
+      <c r="V5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="W5" s="27" t="s">
+      <c r="W5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="X5" s="27" t="s">
+      <c r="X5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="Y5" s="27" t="s">
+      <c r="Y5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="27" t="s">
+      <c r="Z5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="27" t="s">
+      <c r="AA5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AB5" s="27" t="s">
+      <c r="AB5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AC5" s="27" t="s">
+      <c r="AC5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AD5" s="27" t="s">
+      <c r="AD5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="27" t="s">
+      <c r="AE5" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="AF5" s="27" t="s">
+      <c r="AF5" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="AG5" s="27" t="s">
+      <c r="AG5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AH5" s="27" t="s">
+      <c r="AH5" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="AI5" s="27" t="s">
+      <c r="AI5" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="AJ5" s="27" t="s">
+      <c r="AJ5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="AK5" s="27" t="s">
+      <c r="AK5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AL5" s="27" t="s">
+      <c r="AL5" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AM5" s="27" t="s">
+      <c r="AM5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="AN5" s="27" t="s">
+      <c r="AN5" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AO5" s="27" t="s">
+      <c r="AO5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AP5" s="27" t="s">
+      <c r="AP5" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="AQ5" s="27" t="s">
+      <c r="AQ5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AR5" s="27" t="s">
+      <c r="AR5" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AS5" s="27" t="s">
+      <c r="AS5" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="AT5" s="27" t="s">
+      <c r="AT5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="AU5" s="27" t="s">
+      <c r="AU5" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AV5" s="27" t="s">
+      <c r="AV5" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="AW5" s="27" t="s">
+      <c r="AW5" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="AX5" s="27" t="s">
+      <c r="AX5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="AY5" s="27" t="s">
+      <c r="AY5" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="AZ5" s="27" t="s">
+      <c r="AZ5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="BA5" s="27" t="s">
+      <c r="BA5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="BB5" s="27" t="s">
+      <c r="BB5" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="BC5" s="27" t="s">
+      <c r="BC5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="BD5" s="27" t="s">
+      <c r="BD5" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="BE5" s="27" t="s">
+      <c r="BE5" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="BF5" s="27" t="s">
+      <c r="BF5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="BG5" s="27" t="s">
+      <c r="BG5" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="BH5" s="27" t="s">
+      <c r="BH5" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="BI5" s="27" t="s">
+      <c r="BI5" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="BJ5" s="27" t="s">
+      <c r="BJ5" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="BK5" s="27" t="s">
+      <c r="BK5" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="BL5" s="27" t="s">
+      <c r="BL5" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="BM5" s="27" t="s">
+      <c r="BM5" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="BN5" s="27" t="s">
+      <c r="BN5" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="BO5" s="27" t="s">
+      <c r="BO5" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="BP5" s="27" t="s">
+      <c r="BP5" s="26" t="s">
         <v>68</v>
       </c>
       <c r="BQ5" s="1"/>
     </row>
     <row r="6" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B6" s="31">
+      <c r="B6" s="29">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <v>1</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>1</v>
       </c>
       <c r="F6" s="2"/>
@@ -3670,17 +3664,17 @@
       <c r="BP6" s="2"/>
     </row>
     <row r="7" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B7" s="31">
+      <c r="B7" s="29">
         <v>2</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <v>0.5</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="15">
+      <c r="E7" s="20"/>
+      <c r="F7" s="14">
         <v>0.5</v>
       </c>
       <c r="G7" s="2"/>
@@ -3747,17 +3741,17 @@
       <c r="BP7" s="2"/>
     </row>
     <row r="8" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B8" s="31">
+      <c r="B8" s="29">
         <v>3</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <v>0.5</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="15">
+      <c r="E8" s="20"/>
+      <c r="F8" s="14">
         <v>0.5</v>
       </c>
       <c r="G8" s="2"/>
@@ -3824,47 +3818,47 @@
       <c r="BP8" s="2"/>
     </row>
     <row r="9" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B9" s="31">
+      <c r="B9" s="29">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>1</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="21"/>
-      <c r="AH9" s="21"/>
-      <c r="AI9" s="21"/>
-      <c r="AJ9" s="15">
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="20"/>
+      <c r="AJ9" s="14">
         <v>1</v>
       </c>
       <c r="AK9" s="2"/>
@@ -3901,13 +3895,13 @@
       <c r="BP9" s="2"/>
     </row>
     <row r="10" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B10" s="31">
+      <c r="B10" s="29">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>1</v>
       </c>
       <c r="E10" s="2"/>
@@ -3976,49 +3970,49 @@
       <c r="BP10" s="2"/>
     </row>
     <row r="11" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B11" s="31">
+      <c r="B11" s="29">
         <v>6</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>1</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21"/>
-      <c r="AE11" s="21"/>
-      <c r="AF11" s="21"/>
-      <c r="AG11" s="21"/>
-      <c r="AH11" s="21"/>
-      <c r="AI11" s="21"/>
-      <c r="AJ11" s="21"/>
-      <c r="AK11" s="21"/>
-      <c r="AL11" s="15">
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+      <c r="AG11" s="20"/>
+      <c r="AH11" s="20"/>
+      <c r="AI11" s="20"/>
+      <c r="AJ11" s="20"/>
+      <c r="AK11" s="20"/>
+      <c r="AL11" s="14">
         <v>1</v>
       </c>
       <c r="AM11" s="2"/>
@@ -4053,67 +4047,67 @@
       <c r="BP11" s="2"/>
     </row>
     <row r="12" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B12" s="31">
+      <c r="B12" s="29">
         <v>7</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <v>2</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="21"/>
-      <c r="X12" s="21"/>
-      <c r="Y12" s="21"/>
-      <c r="Z12" s="21"/>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
-      <c r="AC12" s="21"/>
-      <c r="AD12" s="21"/>
-      <c r="AE12" s="21"/>
-      <c r="AF12" s="21"/>
-      <c r="AG12" s="21"/>
-      <c r="AH12" s="21"/>
-      <c r="AI12" s="21"/>
-      <c r="AJ12" s="21"/>
-      <c r="AK12" s="17">
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="16">
         <v>1</v>
       </c>
-      <c r="AL12" s="17">
+      <c r="AL12" s="16">
         <v>-1</v>
       </c>
-      <c r="AM12" s="17"/>
-      <c r="AN12" s="17">
+      <c r="AM12" s="16"/>
+      <c r="AN12" s="16">
         <v>1</v>
       </c>
-      <c r="AO12" s="17">
+      <c r="AO12" s="16">
         <v>-1</v>
       </c>
-      <c r="AP12" s="17">
+      <c r="AP12" s="16">
         <v>1</v>
       </c>
-      <c r="AQ12" s="17">
+      <c r="AQ12" s="16">
         <v>-1</v>
       </c>
-      <c r="AR12" s="15">
+      <c r="AR12" s="14">
         <v>2</v>
       </c>
       <c r="AS12" s="2"/>
@@ -4142,13 +4136,13 @@
       <c r="BP12" s="2"/>
     </row>
     <row r="13" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B13" s="31">
+      <c r="B13" s="29">
         <v>8</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>2</v>
       </c>
       <c r="E13" s="2"/>
@@ -4217,13 +4211,13 @@
       <c r="BP13" s="2"/>
     </row>
     <row r="14" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B14" s="31">
+      <c r="B14" s="29">
         <v>9</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>2</v>
       </c>
       <c r="E14" s="2"/>
@@ -4292,13 +4286,13 @@
       <c r="BP14" s="2"/>
     </row>
     <row r="15" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B15" s="31">
+      <c r="B15" s="29">
         <v>10</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>2</v>
       </c>
       <c r="E15" s="2"/>
@@ -4367,13 +4361,13 @@
       <c r="BP15" s="2"/>
     </row>
     <row r="16" spans="2:69" x14ac:dyDescent="0.3">
-      <c r="B16" s="31">
+      <c r="B16" s="29">
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="28">
         <v>1</v>
       </c>
       <c r="E16" s="2"/>
@@ -4442,57 +4436,57 @@
       <c r="BP16" s="2"/>
     </row>
     <row r="17" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B17" s="31">
+      <c r="B17" s="29">
         <v>12</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="14">
         <v>2</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16">
         <v>1</v>
       </c>
-      <c r="Y17" s="17">
+      <c r="Y17" s="16">
         <v>-1</v>
       </c>
-      <c r="Z17" s="17">
+      <c r="Z17" s="16">
         <v>1</v>
       </c>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
-      <c r="AE17" s="21"/>
-      <c r="AF17" s="21"/>
-      <c r="AG17" s="21"/>
-      <c r="AH17" s="21"/>
-      <c r="AI17" s="21"/>
-      <c r="AJ17" s="21"/>
-      <c r="AK17" s="21"/>
-      <c r="AL17" s="21"/>
-      <c r="AM17" s="21"/>
-      <c r="AN17" s="15">
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+      <c r="AI17" s="20"/>
+      <c r="AJ17" s="20"/>
+      <c r="AK17" s="20"/>
+      <c r="AL17" s="20"/>
+      <c r="AM17" s="20"/>
+      <c r="AN17" s="14">
         <v>1</v>
       </c>
       <c r="AO17" s="2"/>
@@ -4525,52 +4519,52 @@
       <c r="BP17" s="2"/>
     </row>
     <row r="18" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B18" s="31">
+      <c r="B18" s="29">
         <v>13</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <v>0.5</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="21"/>
-      <c r="AC18" s="21"/>
-      <c r="AD18" s="21"/>
-      <c r="AE18" s="21"/>
-      <c r="AF18" s="21"/>
-      <c r="AG18" s="21"/>
-      <c r="AH18" s="21"/>
-      <c r="AI18" s="21"/>
-      <c r="AJ18" s="21"/>
-      <c r="AK18" s="21"/>
-      <c r="AL18" s="21"/>
-      <c r="AM18" s="21"/>
-      <c r="AN18" s="21"/>
-      <c r="AO18" s="15">
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+      <c r="AI18" s="20"/>
+      <c r="AJ18" s="20"/>
+      <c r="AK18" s="20"/>
+      <c r="AL18" s="20"/>
+      <c r="AM18" s="20"/>
+      <c r="AN18" s="20"/>
+      <c r="AO18" s="14">
         <v>0.5</v>
       </c>
       <c r="AP18" s="2"/>
@@ -4602,37 +4596,37 @@
       <c r="BP18" s="2"/>
     </row>
     <row r="19" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B19" s="31">
+      <c r="B19" s="29">
         <v>14</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <v>1</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="15">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="14">
         <v>1</v>
       </c>
       <c r="AA19" s="2"/>
@@ -4679,13 +4673,13 @@
       <c r="BP19" s="2"/>
     </row>
     <row r="20" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B20" s="31">
+      <c r="B20" s="29">
         <v>15</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="28">
         <v>0.5</v>
       </c>
       <c r="E20" s="2"/>
@@ -4754,53 +4748,53 @@
       <c r="BP20" s="2"/>
     </row>
     <row r="21" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B21" s="31">
+      <c r="B21" s="29">
         <v>16</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="14">
         <v>2</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
-      <c r="Z21" s="21"/>
-      <c r="AA21" s="21"/>
-      <c r="AB21" s="21"/>
-      <c r="AC21" s="21"/>
-      <c r="AD21" s="21"/>
-      <c r="AE21" s="21"/>
-      <c r="AF21" s="21"/>
-      <c r="AG21" s="21"/>
-      <c r="AH21" s="21"/>
-      <c r="AI21" s="21"/>
-      <c r="AJ21" s="21"/>
-      <c r="AK21" s="21"/>
-      <c r="AL21" s="21"/>
-      <c r="AM21" s="21"/>
-      <c r="AN21" s="21"/>
-      <c r="AO21" s="21"/>
-      <c r="AP21" s="15">
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="20"/>
+      <c r="AA21" s="20"/>
+      <c r="AB21" s="20"/>
+      <c r="AC21" s="20"/>
+      <c r="AD21" s="20"/>
+      <c r="AE21" s="20"/>
+      <c r="AF21" s="20"/>
+      <c r="AG21" s="20"/>
+      <c r="AH21" s="20"/>
+      <c r="AI21" s="20"/>
+      <c r="AJ21" s="20"/>
+      <c r="AK21" s="20"/>
+      <c r="AL21" s="20"/>
+      <c r="AM21" s="20"/>
+      <c r="AN21" s="20"/>
+      <c r="AO21" s="20"/>
+      <c r="AP21" s="14">
         <v>2</v>
       </c>
       <c r="AQ21" s="2"/>
@@ -4831,13 +4825,13 @@
       <c r="BP21" s="2"/>
     </row>
     <row r="22" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B22" s="31">
+      <c r="B22" s="29">
         <v>17</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="28">
         <v>2</v>
       </c>
       <c r="E22" s="2"/>
@@ -4906,13 +4900,13 @@
       <c r="BP22" s="2"/>
     </row>
     <row r="23" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B23" s="31">
+      <c r="B23" s="29">
         <v>18</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="28">
         <v>2</v>
       </c>
       <c r="E23" s="2"/>
@@ -4981,13 +4975,13 @@
       <c r="BP23" s="2"/>
     </row>
     <row r="24" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B24" s="31">
+      <c r="B24" s="29">
         <v>19</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="28">
         <v>2</v>
       </c>
       <c r="E24" s="2"/>
@@ -5056,46 +5050,46 @@
       <c r="BP24" s="2"/>
     </row>
     <row r="25" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B25" s="31">
+      <c r="B25" s="29">
         <v>20</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="14">
         <v>2</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="21"/>
-      <c r="V25" s="21"/>
-      <c r="W25" s="21"/>
-      <c r="X25" s="21"/>
-      <c r="Y25" s="21"/>
-      <c r="Z25" s="21"/>
-      <c r="AA25" s="21"/>
-      <c r="AB25" s="21"/>
-      <c r="AC25" s="21"/>
-      <c r="AD25" s="17">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="20"/>
+      <c r="AA25" s="20"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="20"/>
+      <c r="AD25" s="16">
         <v>1</v>
       </c>
-      <c r="AE25" s="21"/>
-      <c r="AF25" s="21"/>
-      <c r="AG25" s="15">
+      <c r="AE25" s="20"/>
+      <c r="AF25" s="20"/>
+      <c r="AG25" s="14">
         <v>1</v>
       </c>
       <c r="AH25" s="2"/>
@@ -5135,13 +5129,13 @@
       <c r="BP25" s="2"/>
     </row>
     <row r="26" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B26" s="31">
+      <c r="B26" s="29">
         <v>21</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="28">
         <v>2</v>
       </c>
       <c r="E26" s="2"/>
@@ -5210,13 +5204,13 @@
       <c r="BP26" s="2"/>
     </row>
     <row r="27" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B27" s="31">
+      <c r="B27" s="29">
         <v>22</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="28">
         <v>2</v>
       </c>
       <c r="E27" s="2"/>
@@ -5285,13 +5279,13 @@
       <c r="BP27" s="2"/>
     </row>
     <row r="28" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B28" s="31">
+      <c r="B28" s="29">
         <v>23</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="28">
         <v>2</v>
       </c>
       <c r="E28" s="2"/>
@@ -5360,13 +5354,13 @@
       <c r="BP28" s="2"/>
     </row>
     <row r="29" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B29" s="31">
+      <c r="B29" s="29">
         <v>24</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>2</v>
       </c>
       <c r="E29" s="2"/>
@@ -5435,13 +5429,13 @@
       <c r="BP29" s="2"/>
     </row>
     <row r="30" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B30" s="31">
+      <c r="B30" s="29">
         <v>25</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="28">
         <v>2</v>
       </c>
       <c r="E30" s="2"/>
@@ -5510,13 +5504,13 @@
       <c r="BP30" s="2"/>
     </row>
     <row r="31" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B31" s="31">
+      <c r="B31" s="29">
         <v>26</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="28">
         <v>2</v>
       </c>
       <c r="E31" s="2"/>
@@ -5585,13 +5579,13 @@
       <c r="BP31" s="2"/>
     </row>
     <row r="32" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B32" s="31">
+      <c r="B32" s="29">
         <v>27</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="28">
         <v>2</v>
       </c>
       <c r="E32" s="2"/>
@@ -5660,13 +5654,13 @@
       <c r="BP32" s="2"/>
     </row>
     <row r="33" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B33" s="31">
+      <c r="B33" s="29">
         <v>28</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="29">
+      <c r="D33" s="28">
         <v>2</v>
       </c>
       <c r="E33" s="2"/>
@@ -5735,56 +5729,62 @@
       <c r="BP33" s="2"/>
     </row>
     <row r="34" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B34" s="31">
+      <c r="B34" s="29">
         <v>29</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="29">
+      <c r="D34" s="14">
         <v>2</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
-      <c r="AC34" s="2"/>
-      <c r="AD34" s="2"/>
-      <c r="AE34" s="2"/>
-      <c r="AF34" s="2"/>
-      <c r="AG34" s="2"/>
-      <c r="AH34" s="2"/>
-      <c r="AI34" s="2"/>
-      <c r="AJ34" s="2"/>
-      <c r="AK34" s="2"/>
-      <c r="AL34" s="2"/>
-      <c r="AM34" s="2"/>
-      <c r="AN34" s="2"/>
-      <c r="AO34" s="2"/>
-      <c r="AP34" s="2"/>
-      <c r="AQ34" s="2"/>
-      <c r="AR34" s="2"/>
-      <c r="AS34" s="2"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="20"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="20"/>
+      <c r="Y34" s="20"/>
+      <c r="Z34" s="20"/>
+      <c r="AA34" s="20"/>
+      <c r="AB34" s="20"/>
+      <c r="AC34" s="20"/>
+      <c r="AD34" s="20"/>
+      <c r="AE34" s="20"/>
+      <c r="AF34" s="20"/>
+      <c r="AG34" s="20"/>
+      <c r="AH34" s="20"/>
+      <c r="AI34" s="20"/>
+      <c r="AJ34" s="20"/>
+      <c r="AK34" s="20"/>
+      <c r="AL34" s="20"/>
+      <c r="AM34" s="20"/>
+      <c r="AN34" s="20"/>
+      <c r="AO34" s="20"/>
+      <c r="AP34" s="20"/>
+      <c r="AQ34" s="16">
+        <v>1</v>
+      </c>
+      <c r="AR34" s="16">
+        <v>-1</v>
+      </c>
+      <c r="AS34" s="14">
+        <v>2</v>
+      </c>
       <c r="AT34" s="2"/>
       <c r="AU34" s="2"/>
       <c r="AV34" s="2"/>
@@ -5810,13 +5810,13 @@
       <c r="BP34" s="2"/>
     </row>
     <row r="35" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B35" s="31">
+      <c r="B35" s="29">
         <v>30</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="29">
+      <c r="D35" s="28">
         <v>2</v>
       </c>
       <c r="E35" s="2"/>
@@ -5885,56 +5885,58 @@
       <c r="BP35" s="2"/>
     </row>
     <row r="36" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B36" s="31">
+      <c r="B36" s="29">
         <v>31</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D36" s="29">
+      <c r="D36" s="14">
         <v>2</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="2"/>
-      <c r="AD36" s="2"/>
-      <c r="AE36" s="2"/>
-      <c r="AF36" s="2"/>
-      <c r="AG36" s="2"/>
-      <c r="AH36" s="2"/>
-      <c r="AI36" s="2"/>
-      <c r="AJ36" s="2"/>
-      <c r="AK36" s="2"/>
-      <c r="AL36" s="2"/>
-      <c r="AM36" s="2"/>
-      <c r="AN36" s="2"/>
-      <c r="AO36" s="2"/>
-      <c r="AP36" s="2"/>
-      <c r="AQ36" s="2"/>
-      <c r="AR36" s="2"/>
-      <c r="AS36" s="2"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
+      <c r="Z36" s="20"/>
+      <c r="AA36" s="20"/>
+      <c r="AB36" s="20"/>
+      <c r="AC36" s="20"/>
+      <c r="AD36" s="20"/>
+      <c r="AE36" s="20"/>
+      <c r="AF36" s="20"/>
+      <c r="AG36" s="20"/>
+      <c r="AH36" s="20"/>
+      <c r="AI36" s="20"/>
+      <c r="AJ36" s="20"/>
+      <c r="AK36" s="20"/>
+      <c r="AL36" s="20"/>
+      <c r="AM36" s="20"/>
+      <c r="AN36" s="20"/>
+      <c r="AO36" s="20"/>
+      <c r="AP36" s="20"/>
+      <c r="AQ36" s="20"/>
+      <c r="AR36" s="20"/>
+      <c r="AS36" s="14">
+        <v>2</v>
+      </c>
       <c r="AT36" s="2"/>
       <c r="AU36" s="2"/>
       <c r="AV36" s="2"/>
@@ -5960,56 +5962,58 @@
       <c r="BP36" s="2"/>
     </row>
     <row r="37" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B37" s="32">
+      <c r="B37" s="30">
         <v>32</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D37" s="15">
         <v>2</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
-      <c r="U37" s="4"/>
-      <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-      <c r="X37" s="4"/>
-      <c r="Y37" s="4"/>
-      <c r="Z37" s="4"/>
-      <c r="AA37" s="4"/>
-      <c r="AB37" s="4"/>
-      <c r="AC37" s="4"/>
-      <c r="AD37" s="4"/>
-      <c r="AE37" s="4"/>
-      <c r="AF37" s="4"/>
-      <c r="AG37" s="4"/>
-      <c r="AH37" s="4"/>
-      <c r="AI37" s="4"/>
-      <c r="AJ37" s="4"/>
-      <c r="AK37" s="4"/>
-      <c r="AL37" s="4"/>
-      <c r="AM37" s="4"/>
-      <c r="AN37" s="4"/>
-      <c r="AO37" s="4"/>
-      <c r="AP37" s="4"/>
-      <c r="AQ37" s="4"/>
-      <c r="AR37" s="4"/>
-      <c r="AS37" s="4"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="21"/>
+      <c r="Z37" s="21"/>
+      <c r="AA37" s="21"/>
+      <c r="AB37" s="21"/>
+      <c r="AC37" s="21"/>
+      <c r="AD37" s="21"/>
+      <c r="AE37" s="21"/>
+      <c r="AF37" s="21"/>
+      <c r="AG37" s="21"/>
+      <c r="AH37" s="21"/>
+      <c r="AI37" s="21"/>
+      <c r="AJ37" s="21"/>
+      <c r="AK37" s="21"/>
+      <c r="AL37" s="21"/>
+      <c r="AM37" s="21"/>
+      <c r="AN37" s="21"/>
+      <c r="AO37" s="21"/>
+      <c r="AP37" s="21"/>
+      <c r="AQ37" s="21"/>
+      <c r="AR37" s="21"/>
+      <c r="AS37" s="15">
+        <v>2</v>
+      </c>
       <c r="AT37" s="4"/>
       <c r="AU37" s="4"/>
       <c r="AV37" s="4"/>
@@ -6035,37 +6039,37 @@
       <c r="BP37" s="4"/>
     </row>
     <row r="38" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B38" s="33">
+      <c r="B38" s="31">
         <v>33</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="15">
         <v>1</v>
       </c>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="22"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-      <c r="T38" s="22"/>
-      <c r="U38" s="22"/>
-      <c r="V38" s="22"/>
-      <c r="W38" s="22"/>
-      <c r="X38" s="22"/>
-      <c r="Y38" s="22"/>
-      <c r="Z38" s="16">
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="21"/>
+      <c r="Z38" s="15">
         <v>1</v>
       </c>
       <c r="AA38" s="4"/>
@@ -6112,51 +6116,51 @@
       <c r="BP38" s="4"/>
     </row>
     <row r="39" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B39" s="32">
+      <c r="B39" s="30">
         <v>34</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="14">
         <v>1</v>
       </c>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="21"/>
-      <c r="AA39" s="21"/>
-      <c r="AB39" s="21"/>
-      <c r="AC39" s="21"/>
-      <c r="AD39" s="21"/>
-      <c r="AE39" s="21"/>
-      <c r="AF39" s="21"/>
-      <c r="AG39" s="21"/>
-      <c r="AH39" s="21"/>
-      <c r="AI39" s="21"/>
-      <c r="AJ39" s="21"/>
-      <c r="AK39" s="21"/>
-      <c r="AL39" s="21"/>
-      <c r="AM39" s="21"/>
-      <c r="AN39" s="15">
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="20"/>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="20"/>
+      <c r="T39" s="20"/>
+      <c r="U39" s="20"/>
+      <c r="V39" s="20"/>
+      <c r="W39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="20"/>
+      <c r="AE39" s="20"/>
+      <c r="AF39" s="20"/>
+      <c r="AG39" s="20"/>
+      <c r="AH39" s="20"/>
+      <c r="AI39" s="20"/>
+      <c r="AJ39" s="20"/>
+      <c r="AK39" s="20"/>
+      <c r="AL39" s="20"/>
+      <c r="AM39" s="20"/>
+      <c r="AN39" s="14">
         <v>1</v>
       </c>
       <c r="AO39" s="2"/>
@@ -6189,50 +6193,50 @@
       <c r="BP39" s="2"/>
     </row>
     <row r="40" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B40" s="33">
+      <c r="B40" s="31">
         <v>35</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="14">
         <v>1</v>
       </c>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
-      <c r="V40" s="21"/>
-      <c r="W40" s="21"/>
-      <c r="X40" s="21"/>
-      <c r="Y40" s="21"/>
-      <c r="Z40" s="21"/>
-      <c r="AA40" s="21"/>
-      <c r="AB40" s="21"/>
-      <c r="AC40" s="21"/>
-      <c r="AD40" s="21"/>
-      <c r="AE40" s="21"/>
-      <c r="AF40" s="21"/>
-      <c r="AG40" s="21"/>
-      <c r="AH40" s="21"/>
-      <c r="AI40" s="21"/>
-      <c r="AJ40" s="21"/>
-      <c r="AK40" s="21"/>
-      <c r="AL40" s="21"/>
-      <c r="AM40" s="15">
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="20"/>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="20"/>
+      <c r="T40" s="20"/>
+      <c r="U40" s="20"/>
+      <c r="V40" s="20"/>
+      <c r="W40" s="20"/>
+      <c r="X40" s="20"/>
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="20"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="20"/>
+      <c r="AE40" s="20"/>
+      <c r="AF40" s="20"/>
+      <c r="AG40" s="20"/>
+      <c r="AH40" s="20"/>
+      <c r="AI40" s="20"/>
+      <c r="AJ40" s="20"/>
+      <c r="AK40" s="20"/>
+      <c r="AL40" s="20"/>
+      <c r="AM40" s="14">
         <v>1</v>
       </c>
       <c r="AN40" s="2"/>
@@ -6266,51 +6270,51 @@
       <c r="BP40" s="2"/>
     </row>
     <row r="41" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B41" s="32">
+      <c r="B41" s="30">
         <v>36</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="14">
         <v>1</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
-      <c r="V41" s="21"/>
-      <c r="W41" s="21"/>
-      <c r="X41" s="21"/>
-      <c r="Y41" s="21"/>
-      <c r="Z41" s="21"/>
-      <c r="AA41" s="21"/>
-      <c r="AB41" s="21"/>
-      <c r="AC41" s="21"/>
-      <c r="AD41" s="21"/>
-      <c r="AE41" s="21"/>
-      <c r="AF41" s="21"/>
-      <c r="AG41" s="21"/>
-      <c r="AH41" s="21"/>
-      <c r="AI41" s="21"/>
-      <c r="AJ41" s="21"/>
-      <c r="AK41" s="21"/>
-      <c r="AL41" s="21"/>
-      <c r="AM41" s="21"/>
-      <c r="AN41" s="15">
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="20"/>
+      <c r="T41" s="20"/>
+      <c r="U41" s="20"/>
+      <c r="V41" s="20"/>
+      <c r="W41" s="20"/>
+      <c r="X41" s="20"/>
+      <c r="Y41" s="20"/>
+      <c r="Z41" s="20"/>
+      <c r="AA41" s="20"/>
+      <c r="AB41" s="20"/>
+      <c r="AC41" s="20"/>
+      <c r="AD41" s="20"/>
+      <c r="AE41" s="20"/>
+      <c r="AF41" s="20"/>
+      <c r="AG41" s="20"/>
+      <c r="AH41" s="20"/>
+      <c r="AI41" s="20"/>
+      <c r="AJ41" s="20"/>
+      <c r="AK41" s="20"/>
+      <c r="AL41" s="20"/>
+      <c r="AM41" s="20"/>
+      <c r="AN41" s="14">
         <v>1</v>
       </c>
       <c r="AO41" s="2"/>
@@ -6343,47 +6347,47 @@
       <c r="BP41" s="2"/>
     </row>
     <row r="42" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B42" s="33">
+      <c r="B42" s="31">
         <v>37</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="14">
         <v>1</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
-      <c r="O42" s="21"/>
-      <c r="P42" s="21"/>
-      <c r="Q42" s="21"/>
-      <c r="R42" s="21"/>
-      <c r="S42" s="21"/>
-      <c r="T42" s="21"/>
-      <c r="U42" s="21"/>
-      <c r="V42" s="21"/>
-      <c r="W42" s="21"/>
-      <c r="X42" s="21"/>
-      <c r="Y42" s="21"/>
-      <c r="Z42" s="21"/>
-      <c r="AA42" s="21"/>
-      <c r="AB42" s="21"/>
-      <c r="AC42" s="21"/>
-      <c r="AD42" s="21"/>
-      <c r="AE42" s="21"/>
-      <c r="AF42" s="21"/>
-      <c r="AG42" s="21"/>
-      <c r="AH42" s="21"/>
-      <c r="AI42" s="21"/>
-      <c r="AJ42" s="15">
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="20"/>
+      <c r="AA42" s="20"/>
+      <c r="AB42" s="20"/>
+      <c r="AC42" s="20"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="20"/>
+      <c r="AF42" s="20"/>
+      <c r="AG42" s="20"/>
+      <c r="AH42" s="20"/>
+      <c r="AI42" s="20"/>
+      <c r="AJ42" s="14">
         <v>1</v>
       </c>
       <c r="AK42" s="2"/>
@@ -6420,13 +6424,13 @@
       <c r="BP42" s="2"/>
     </row>
     <row r="43" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B43" s="32">
+      <c r="B43" s="30">
         <v>38</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43" s="28">
         <v>4</v>
       </c>
       <c r="E43" s="2"/>
@@ -6495,51 +6499,51 @@
       <c r="BP43" s="2"/>
     </row>
     <row r="44" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B44" s="33">
+      <c r="B44" s="31">
         <v>39</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="14">
         <v>1</v>
       </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
-      <c r="N44" s="21"/>
-      <c r="O44" s="21"/>
-      <c r="P44" s="21"/>
-      <c r="Q44" s="21"/>
-      <c r="R44" s="21"/>
-      <c r="S44" s="21"/>
-      <c r="T44" s="21"/>
-      <c r="U44" s="21"/>
-      <c r="V44" s="21"/>
-      <c r="W44" s="21"/>
-      <c r="X44" s="21"/>
-      <c r="Y44" s="21"/>
-      <c r="Z44" s="21"/>
-      <c r="AA44" s="21"/>
-      <c r="AB44" s="21"/>
-      <c r="AC44" s="21"/>
-      <c r="AD44" s="21"/>
-      <c r="AE44" s="21"/>
-      <c r="AF44" s="21"/>
-      <c r="AG44" s="21"/>
-      <c r="AH44" s="21"/>
-      <c r="AI44" s="21"/>
-      <c r="AJ44" s="21"/>
-      <c r="AK44" s="21"/>
-      <c r="AL44" s="21"/>
-      <c r="AM44" s="21"/>
-      <c r="AN44" s="15">
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="20"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="20"/>
+      <c r="AF44" s="20"/>
+      <c r="AG44" s="20"/>
+      <c r="AH44" s="20"/>
+      <c r="AI44" s="20"/>
+      <c r="AJ44" s="20"/>
+      <c r="AK44" s="20"/>
+      <c r="AL44" s="20"/>
+      <c r="AM44" s="20"/>
+      <c r="AN44" s="14">
         <v>1</v>
       </c>
       <c r="AO44" s="2"/>
@@ -6572,11 +6576,11 @@
       <c r="BP44" s="2"/>
     </row>
     <row r="45" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B45" s="32">
+      <c r="B45" s="30">
         <v>40</v>
       </c>
       <c r="C45" s="3"/>
-      <c r="D45" s="29">
+      <c r="D45" s="28">
         <v>1</v>
       </c>
       <c r="E45" s="2"/>
@@ -6645,11 +6649,11 @@
       <c r="BP45" s="2"/>
     </row>
     <row r="46" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B46" s="33">
+      <c r="B46" s="31">
         <v>41</v>
       </c>
       <c r="C46" s="3"/>
-      <c r="D46" s="29">
+      <c r="D46" s="28">
         <v>1</v>
       </c>
       <c r="E46" s="2"/>
@@ -6718,9 +6722,9 @@
       <c r="BP46" s="2"/>
     </row>
     <row r="47" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -6787,9 +6791,9 @@
       <c r="BP47" s="2"/>
     </row>
     <row r="48" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="26"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="25"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -6856,10 +6860,10 @@
       <c r="BP48" s="4"/>
     </row>
     <row r="49" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="39"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="5">
         <f>SUM(D6:D48)</f>
         <v>64</v>
@@ -7018,7 +7022,7 @@
       </c>
       <c r="AQ49" s="5">
         <f t="shared" ref="AQ49" si="27">AP49-SUM(AQ6:AQ48)</f>
-        <v>46.5</v>
+        <v>45.5</v>
       </c>
       <c r="AR49" s="5">
         <f t="shared" ref="AR49" si="28">AQ49-SUM(AR6:AR48)</f>
@@ -7026,106 +7030,106 @@
       </c>
       <c r="AS49" s="5">
         <f t="shared" ref="AS49" si="29">AR49-SUM(AS6:AS48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="AT49" s="5">
         <f t="shared" ref="AT49" si="30">AS49-SUM(AT6:AT48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="AU49" s="5">
         <f t="shared" ref="AU49" si="31">AT49-SUM(AU6:AU48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="AV49" s="5">
         <f t="shared" ref="AV49" si="32">AU49-SUM(AV6:AV48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="AW49" s="5">
         <f t="shared" ref="AW49" si="33">AV49-SUM(AW6:AW48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="AX49" s="5">
         <f t="shared" ref="AX49" si="34">AW49-SUM(AX6:AX48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="AY49" s="5">
         <f t="shared" ref="AY49" si="35">AX49-SUM(AY6:AY48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="AZ49" s="5">
         <f>AY49-SUM(AZ6:AZ48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BA49" s="5">
         <f t="shared" ref="BA49" si="36">AZ49-SUM(BA6:BA48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BB49" s="5">
         <f t="shared" ref="BB49" si="37">BA49-SUM(BB6:BB48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BC49" s="5">
         <f t="shared" ref="BC49" si="38">BB49-SUM(BC6:BC48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BD49" s="5">
         <f t="shared" ref="BD49" si="39">BC49-SUM(BD6:BD48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BE49" s="5">
         <f t="shared" ref="BE49" si="40">BD49-SUM(BE6:BE48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BF49" s="5">
         <f t="shared" ref="BF49" si="41">BE49-SUM(BF6:BF48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BG49" s="5">
         <f t="shared" ref="BG49" si="42">BF49-SUM(BG6:BG48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BH49" s="5">
         <f t="shared" ref="BH49" si="43">BG49-SUM(BH6:BH48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BI49" s="5">
         <f t="shared" ref="BI49" si="44">BH49-SUM(BI6:BI48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BJ49" s="5">
         <f t="shared" ref="BJ49" si="45">BI49-SUM(BJ6:BJ48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BK49" s="5">
         <f t="shared" ref="BK49" si="46">BJ49-SUM(BK6:BK48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BL49" s="5">
         <f t="shared" ref="BL49" si="47">BK49-SUM(BL6:BL48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BM49" s="5">
         <f t="shared" ref="BM49" si="48">BL49-SUM(BM6:BM48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BN49" s="5">
         <f t="shared" ref="BN49" si="49">BM49-SUM(BN6:BN48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
       <c r="BO49" s="5">
         <f>BN49-SUM(BO6:BO48)</f>
-        <v>44.5</v>
-      </c>
-      <c r="BP49" s="13">
+        <v>38.5</v>
+      </c>
+      <c r="BP49" s="12">
         <f t="shared" ref="BP49" si="50">BO49-SUM(BP6:BP48)</f>
-        <v>44.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="50" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="37"/>
+      <c r="C50" s="35"/>
       <c r="D50" s="6">
         <f>SUM(D6:D48)</f>
         <v>64</v>
@@ -7382,23 +7386,23 @@
         <f>$D$50-($D$50/64*63)</f>
         <v>1</v>
       </c>
-      <c r="BP50" s="14">
+      <c r="BP50" s="13">
         <f>$D$50-($D$50/64*64)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:68" x14ac:dyDescent="0.3">
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="18" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="19" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
login functionality repaired, naming changes
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB04138-567D-4D33-A957-A57717D2E6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC203CD2-6435-4894-9BF3-365F803FEA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1337,70 +1337,70 @@
                   <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>36.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3019,21 +3019,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="39" max="40" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="39" max="40" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:69" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:69" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
@@ -3105,7 +3105,7 @@
       <c r="BP2" s="31"/>
       <c r="BQ2" s="1"/>
     </row>
-    <row r="3" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
       <c r="D3" s="42"/>
@@ -3174,7 +3174,7 @@
       <c r="BO3" s="3"/>
       <c r="BP3" s="3"/>
     </row>
-    <row r="4" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B4" s="37" t="s">
         <v>1</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
       <c r="D5" s="25" t="s">
@@ -3577,7 +3577,7 @@
       </c>
       <c r="BQ5" s="1"/>
     </row>
-    <row r="6" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B6" s="28">
         <v>1</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="BO6" s="2"/>
       <c r="BP6" s="2"/>
     </row>
-    <row r="7" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B7" s="28">
         <v>2</v>
       </c>
@@ -3731,7 +3731,7 @@
       <c r="BO7" s="2"/>
       <c r="BP7" s="2"/>
     </row>
-    <row r="8" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B8" s="28">
         <v>3</v>
       </c>
@@ -3808,7 +3808,7 @@
       <c r="BO8" s="2"/>
       <c r="BP8" s="2"/>
     </row>
-    <row r="9" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B9" s="28">
         <v>4</v>
       </c>
@@ -3885,7 +3885,7 @@
       <c r="BO9" s="2"/>
       <c r="BP9" s="2"/>
     </row>
-    <row r="10" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B10" s="28">
         <v>5</v>
       </c>
@@ -3960,7 +3960,7 @@
       <c r="BO10" s="2"/>
       <c r="BP10" s="2"/>
     </row>
-    <row r="11" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B11" s="28">
         <v>6</v>
       </c>
@@ -4037,7 +4037,7 @@
       <c r="BO11" s="2"/>
       <c r="BP11" s="2"/>
     </row>
-    <row r="12" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B12" s="28">
         <v>7</v>
       </c>
@@ -4126,59 +4126,61 @@
       <c r="BO12" s="2"/>
       <c r="BP12" s="2"/>
     </row>
-    <row r="13" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B13" s="28">
         <v>8</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="15">
         <v>2</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2"/>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="2"/>
-      <c r="AP13" s="2"/>
-      <c r="AQ13" s="2"/>
-      <c r="AR13" s="2"/>
-      <c r="AS13" s="2"/>
-      <c r="AT13" s="2"/>
-      <c r="AU13" s="2"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="15"/>
+      <c r="AJ13" s="15"/>
+      <c r="AK13" s="15"/>
+      <c r="AL13" s="15"/>
+      <c r="AM13" s="15"/>
+      <c r="AN13" s="15"/>
+      <c r="AO13" s="15"/>
+      <c r="AP13" s="15"/>
+      <c r="AQ13" s="15"/>
+      <c r="AR13" s="15"/>
+      <c r="AS13" s="15"/>
+      <c r="AT13" s="15"/>
+      <c r="AU13" s="15">
+        <v>1</v>
+      </c>
       <c r="AV13" s="2"/>
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
@@ -4201,7 +4203,7 @@
       <c r="BO13" s="2"/>
       <c r="BP13" s="2"/>
     </row>
-    <row r="14" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B14" s="28">
         <v>9</v>
       </c>
@@ -4276,7 +4278,7 @@
       <c r="BO14" s="2"/>
       <c r="BP14" s="2"/>
     </row>
-    <row r="15" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B15" s="28">
         <v>10</v>
       </c>
@@ -4351,7 +4353,7 @@
       <c r="BO15" s="2"/>
       <c r="BP15" s="2"/>
     </row>
-    <row r="16" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B16" s="28">
         <v>11</v>
       </c>
@@ -4426,7 +4428,7 @@
       <c r="BO16" s="2"/>
       <c r="BP16" s="2"/>
     </row>
-    <row r="17" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B17" s="28">
         <v>12</v>
       </c>
@@ -4509,7 +4511,7 @@
       <c r="BO17" s="2"/>
       <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B18" s="28">
         <v>13</v>
       </c>
@@ -4586,7 +4588,7 @@
       <c r="BO18" s="2"/>
       <c r="BP18" s="2"/>
     </row>
-    <row r="19" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B19" s="28">
         <v>14</v>
       </c>
@@ -4663,7 +4665,7 @@
       <c r="BO19" s="2"/>
       <c r="BP19" s="2"/>
     </row>
-    <row r="20" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B20" s="28">
         <v>15</v>
       </c>
@@ -4738,7 +4740,7 @@
       <c r="BO20" s="2"/>
       <c r="BP20" s="2"/>
     </row>
-    <row r="21" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B21" s="28">
         <v>16</v>
       </c>
@@ -4815,7 +4817,7 @@
       <c r="BO21" s="2"/>
       <c r="BP21" s="2"/>
     </row>
-    <row r="22" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B22" s="28">
         <v>17</v>
       </c>
@@ -4890,7 +4892,7 @@
       <c r="BO22" s="2"/>
       <c r="BP22" s="2"/>
     </row>
-    <row r="23" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B23" s="28">
         <v>18</v>
       </c>
@@ -4965,7 +4967,7 @@
       <c r="BO23" s="2"/>
       <c r="BP23" s="2"/>
     </row>
-    <row r="24" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B24" s="28">
         <v>19</v>
       </c>
@@ -5040,7 +5042,7 @@
       <c r="BO24" s="2"/>
       <c r="BP24" s="2"/>
     </row>
-    <row r="25" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B25" s="28">
         <v>20</v>
       </c>
@@ -5119,7 +5121,7 @@
       <c r="BO25" s="2"/>
       <c r="BP25" s="2"/>
     </row>
-    <row r="26" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B26" s="28">
         <v>21</v>
       </c>
@@ -5194,7 +5196,7 @@
       <c r="BO26" s="2"/>
       <c r="BP26" s="2"/>
     </row>
-    <row r="27" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B27" s="28">
         <v>22</v>
       </c>
@@ -5269,7 +5271,7 @@
       <c r="BO27" s="2"/>
       <c r="BP27" s="2"/>
     </row>
-    <row r="28" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B28" s="28">
         <v>23</v>
       </c>
@@ -5344,7 +5346,7 @@
       <c r="BO28" s="2"/>
       <c r="BP28" s="2"/>
     </row>
-    <row r="29" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B29" s="28">
         <v>24</v>
       </c>
@@ -5419,7 +5421,7 @@
       <c r="BO29" s="2"/>
       <c r="BP29" s="2"/>
     </row>
-    <row r="30" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B30" s="28">
         <v>25</v>
       </c>
@@ -5494,7 +5496,7 @@
       <c r="BO30" s="2"/>
       <c r="BP30" s="2"/>
     </row>
-    <row r="31" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B31" s="28">
         <v>26</v>
       </c>
@@ -5569,7 +5571,7 @@
       <c r="BO31" s="2"/>
       <c r="BP31" s="2"/>
     </row>
-    <row r="32" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B32" s="28">
         <v>27</v>
       </c>
@@ -5644,7 +5646,7 @@
       <c r="BO32" s="2"/>
       <c r="BP32" s="2"/>
     </row>
-    <row r="33" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B33" s="28">
         <v>28</v>
       </c>
@@ -5719,7 +5721,7 @@
       <c r="BO33" s="2"/>
       <c r="BP33" s="2"/>
     </row>
-    <row r="34" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B34" s="28">
         <v>29</v>
       </c>
@@ -5800,7 +5802,7 @@
       <c r="BO34" s="2"/>
       <c r="BP34" s="2"/>
     </row>
-    <row r="35" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B35" s="28">
         <v>30</v>
       </c>
@@ -5877,7 +5879,7 @@
       <c r="BO35" s="2"/>
       <c r="BP35" s="2"/>
     </row>
-    <row r="36" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B36" s="28">
         <v>31</v>
       </c>
@@ -5954,7 +5956,7 @@
       <c r="BO36" s="2"/>
       <c r="BP36" s="2"/>
     </row>
-    <row r="37" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B37" s="29">
         <v>32</v>
       </c>
@@ -6031,7 +6033,7 @@
       <c r="BO37" s="4"/>
       <c r="BP37" s="4"/>
     </row>
-    <row r="38" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B38" s="30">
         <v>33</v>
       </c>
@@ -6108,7 +6110,7 @@
       <c r="BO38" s="4"/>
       <c r="BP38" s="4"/>
     </row>
-    <row r="39" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B39" s="29">
         <v>34</v>
       </c>
@@ -6185,7 +6187,7 @@
       <c r="BO39" s="2"/>
       <c r="BP39" s="2"/>
     </row>
-    <row r="40" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B40" s="30">
         <v>35</v>
       </c>
@@ -6262,7 +6264,7 @@
       <c r="BO40" s="2"/>
       <c r="BP40" s="2"/>
     </row>
-    <row r="41" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B41" s="29">
         <v>36</v>
       </c>
@@ -6339,7 +6341,7 @@
       <c r="BO41" s="2"/>
       <c r="BP41" s="2"/>
     </row>
-    <row r="42" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B42" s="30">
         <v>37</v>
       </c>
@@ -6416,7 +6418,7 @@
       <c r="BO42" s="2"/>
       <c r="BP42" s="2"/>
     </row>
-    <row r="43" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B43" s="29">
         <v>38</v>
       </c>
@@ -6491,7 +6493,7 @@
       <c r="BO43" s="2"/>
       <c r="BP43" s="2"/>
     </row>
-    <row r="44" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B44" s="30">
         <v>39</v>
       </c>
@@ -6568,7 +6570,7 @@
       <c r="BO44" s="2"/>
       <c r="BP44" s="2"/>
     </row>
-    <row r="45" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B45" s="29">
         <v>40</v>
       </c>
@@ -6641,7 +6643,7 @@
       <c r="BO45" s="2"/>
       <c r="BP45" s="2"/>
     </row>
-    <row r="46" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B46" s="30">
         <v>41</v>
       </c>
@@ -6714,7 +6716,7 @@
       <c r="BO46" s="2"/>
       <c r="BP46" s="2"/>
     </row>
-    <row r="47" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
       <c r="D47" s="22"/>
@@ -6783,7 +6785,7 @@
       <c r="BO47" s="2"/>
       <c r="BP47" s="2"/>
     </row>
-    <row r="48" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B48" s="23"/>
       <c r="C48" s="23"/>
       <c r="D48" s="24"/>
@@ -6852,7 +6854,7 @@
       <c r="BO48" s="4"/>
       <c r="BP48" s="4"/>
     </row>
-    <row r="49" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B49" s="35" t="s">
         <v>69</v>
       </c>
@@ -7031,94 +7033,94 @@
       </c>
       <c r="AU49" s="5">
         <f t="shared" ref="AU49" si="31">AT49-SUM(AU6:AU48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="AV49" s="5">
         <f t="shared" ref="AV49" si="32">AU49-SUM(AV6:AV48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="AW49" s="5">
         <f t="shared" ref="AW49" si="33">AV49-SUM(AW6:AW48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="AX49" s="5">
         <f t="shared" ref="AX49" si="34">AW49-SUM(AX6:AX48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="AY49" s="5">
         <f t="shared" ref="AY49" si="35">AX49-SUM(AY6:AY48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="AZ49" s="5">
         <f>AY49-SUM(AZ6:AZ48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BA49" s="5">
         <f t="shared" ref="BA49" si="36">AZ49-SUM(BA6:BA48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BB49" s="5">
         <f t="shared" ref="BB49" si="37">BA49-SUM(BB6:BB48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BC49" s="5">
         <f t="shared" ref="BC49" si="38">BB49-SUM(BC6:BC48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BD49" s="5">
         <f t="shared" ref="BD49" si="39">BC49-SUM(BD6:BD48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BE49" s="5">
         <f t="shared" ref="BE49" si="40">BD49-SUM(BE6:BE48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BF49" s="5">
         <f t="shared" ref="BF49" si="41">BE49-SUM(BF6:BF48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BG49" s="5">
         <f t="shared" ref="BG49" si="42">BF49-SUM(BG6:BG48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BH49" s="5">
         <f t="shared" ref="BH49" si="43">BG49-SUM(BH6:BH48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BI49" s="5">
         <f t="shared" ref="BI49" si="44">BH49-SUM(BI6:BI48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BJ49" s="5">
         <f t="shared" ref="BJ49" si="45">BI49-SUM(BJ6:BJ48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BK49" s="5">
         <f t="shared" ref="BK49" si="46">BJ49-SUM(BK6:BK48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BL49" s="5">
         <f t="shared" ref="BL49" si="47">BK49-SUM(BL6:BL48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BM49" s="5">
         <f t="shared" ref="BM49" si="48">BL49-SUM(BM6:BM48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BN49" s="5">
         <f t="shared" ref="BN49" si="49">BM49-SUM(BN6:BN48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BO49" s="5">
         <f>BN49-SUM(BO6:BO48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
       <c r="BP49" s="11">
         <f t="shared" ref="BP49" si="50">BO49-SUM(BP6:BP48)</f>
-        <v>36.5</v>
+        <v>35.5</v>
       </c>
     </row>
-    <row r="50" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B50" s="33" t="s">
         <v>70</v>
       </c>
@@ -7384,17 +7386,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B51" s="16" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B52" s="17" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B53" s="18" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
flexibility adjustment for view.RowInfo
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C2B19B-7ED5-46F8-B0EF-BE0429533C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD31F206-063E-4B02-A060-5FA43F9DDD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -883,8 +883,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF99"/>
       <color rgb="FFCCFFCC"/>
-      <color rgb="FF99FF99"/>
       <color rgb="FF33CC33"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFF0066"/>
@@ -1351,67 +1351,67 @@
                   <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>30.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3030,21 +3030,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AV23" sqref="AV23"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="AW13" sqref="AW13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="39" max="40" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.08984375" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="39" max="40" width="9.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:69" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:69" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
@@ -3116,7 +3116,7 @@
       <c r="BP2" s="34"/>
       <c r="BQ2" s="1"/>
     </row>
-    <row r="3" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
@@ -3185,7 +3185,7 @@
       <c r="BO3" s="3"/>
       <c r="BP3" s="3"/>
     </row>
-    <row r="4" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B4" s="36" t="s">
         <v>1</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
       <c r="D5" s="18" t="s">
@@ -3588,7 +3588,7 @@
       </c>
       <c r="BQ5" s="1"/>
     </row>
-    <row r="6" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B6" s="21">
         <v>1</v>
       </c>
@@ -3665,7 +3665,7 @@
       <c r="BO6" s="2"/>
       <c r="BP6" s="2"/>
     </row>
-    <row r="7" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B7" s="21">
         <v>2</v>
       </c>
@@ -3742,7 +3742,7 @@
       <c r="BO7" s="2"/>
       <c r="BP7" s="2"/>
     </row>
-    <row r="8" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B8" s="21">
         <v>3</v>
       </c>
@@ -3819,7 +3819,7 @@
       <c r="BO8" s="2"/>
       <c r="BP8" s="2"/>
     </row>
-    <row r="9" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B9" s="21">
         <v>4</v>
       </c>
@@ -3896,7 +3896,7 @@
       <c r="BO9" s="2"/>
       <c r="BP9" s="2"/>
     </row>
-    <row r="10" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B10" s="21">
         <v>5</v>
       </c>
@@ -3973,7 +3973,7 @@
       <c r="BO10" s="2"/>
       <c r="BP10" s="2"/>
     </row>
-    <row r="11" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B11" s="21">
         <v>6</v>
       </c>
@@ -4050,7 +4050,7 @@
       <c r="BO11" s="2"/>
       <c r="BP11" s="2"/>
     </row>
-    <row r="12" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B12" s="21">
         <v>7</v>
       </c>
@@ -4139,62 +4139,64 @@
       <c r="BO12" s="2"/>
       <c r="BP12" s="2"/>
     </row>
-    <row r="13" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B13" s="21">
         <v>8</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="10">
         <v>2</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="12"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="12"/>
-      <c r="AM13" s="12"/>
-      <c r="AN13" s="12"/>
-      <c r="AO13" s="12"/>
-      <c r="AP13" s="12"/>
-      <c r="AQ13" s="12"/>
-      <c r="AR13" s="12"/>
-      <c r="AS13" s="12"/>
-      <c r="AT13" s="12"/>
-      <c r="AU13" s="12">
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="16"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="16"/>
+      <c r="AF13" s="16"/>
+      <c r="AG13" s="16"/>
+      <c r="AH13" s="16"/>
+      <c r="AI13" s="16"/>
+      <c r="AJ13" s="16"/>
+      <c r="AK13" s="16"/>
+      <c r="AL13" s="16"/>
+      <c r="AM13" s="16"/>
+      <c r="AN13" s="16"/>
+      <c r="AO13" s="16"/>
+      <c r="AP13" s="16"/>
+      <c r="AQ13" s="16"/>
+      <c r="AR13" s="16"/>
+      <c r="AS13" s="16"/>
+      <c r="AT13" s="16"/>
+      <c r="AU13" s="10">
         <v>1</v>
       </c>
-      <c r="AV13" s="2"/>
+      <c r="AV13" s="10">
+        <v>1</v>
+      </c>
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
@@ -4216,7 +4218,7 @@
       <c r="BO13" s="2"/>
       <c r="BP13" s="2"/>
     </row>
-    <row r="14" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B14" s="21">
         <v>9</v>
       </c>
@@ -4293,7 +4295,7 @@
       <c r="BO14" s="2"/>
       <c r="BP14" s="2"/>
     </row>
-    <row r="15" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B15" s="21">
         <v>10</v>
       </c>
@@ -4370,7 +4372,7 @@
       <c r="BO15" s="2"/>
       <c r="BP15" s="2"/>
     </row>
-    <row r="16" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:69" x14ac:dyDescent="0.35">
       <c r="B16" s="21">
         <v>11</v>
       </c>
@@ -4445,7 +4447,7 @@
       <c r="BO16" s="2"/>
       <c r="BP16" s="2"/>
     </row>
-    <row r="17" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B17" s="21">
         <v>12</v>
       </c>
@@ -4528,7 +4530,7 @@
       <c r="BO17" s="2"/>
       <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B18" s="21">
         <v>13</v>
       </c>
@@ -4605,7 +4607,7 @@
       <c r="BO18" s="2"/>
       <c r="BP18" s="2"/>
     </row>
-    <row r="19" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B19" s="21">
         <v>14</v>
       </c>
@@ -4686,7 +4688,7 @@
       <c r="BO19" s="2"/>
       <c r="BP19" s="2"/>
     </row>
-    <row r="20" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B20" s="21">
         <v>15</v>
       </c>
@@ -4763,7 +4765,7 @@
       <c r="BO20" s="2"/>
       <c r="BP20" s="2"/>
     </row>
-    <row r="21" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B21" s="21">
         <v>16</v>
       </c>
@@ -4840,7 +4842,7 @@
       <c r="BO21" s="2"/>
       <c r="BP21" s="2"/>
     </row>
-    <row r="22" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B22" s="21">
         <v>17</v>
       </c>
@@ -4915,7 +4917,7 @@
       <c r="BO22" s="2"/>
       <c r="BP22" s="2"/>
     </row>
-    <row r="23" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B23" s="21">
         <v>18</v>
       </c>
@@ -4990,7 +4992,7 @@
       <c r="BO23" s="2"/>
       <c r="BP23" s="2"/>
     </row>
-    <row r="24" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B24" s="21">
         <v>19</v>
       </c>
@@ -5065,7 +5067,7 @@
       <c r="BO24" s="2"/>
       <c r="BP24" s="2"/>
     </row>
-    <row r="25" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B25" s="21">
         <v>20</v>
       </c>
@@ -5144,7 +5146,7 @@
       <c r="BO25" s="2"/>
       <c r="BP25" s="2"/>
     </row>
-    <row r="26" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B26" s="21">
         <v>21</v>
       </c>
@@ -5219,7 +5221,7 @@
       <c r="BO26" s="2"/>
       <c r="BP26" s="2"/>
     </row>
-    <row r="27" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B27" s="21">
         <v>22</v>
       </c>
@@ -5296,7 +5298,7 @@
       <c r="BO27" s="2"/>
       <c r="BP27" s="2"/>
     </row>
-    <row r="28" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B28" s="21">
         <v>23</v>
       </c>
@@ -5371,7 +5373,7 @@
       <c r="BO28" s="2"/>
       <c r="BP28" s="2"/>
     </row>
-    <row r="29" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B29" s="21">
         <v>24</v>
       </c>
@@ -5446,7 +5448,7 @@
       <c r="BO29" s="2"/>
       <c r="BP29" s="2"/>
     </row>
-    <row r="30" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B30" s="21">
         <v>25</v>
       </c>
@@ -5521,7 +5523,7 @@
       <c r="BO30" s="2"/>
       <c r="BP30" s="2"/>
     </row>
-    <row r="31" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B31" s="21">
         <v>26</v>
       </c>
@@ -5598,7 +5600,7 @@
       <c r="BO31" s="2"/>
       <c r="BP31" s="2"/>
     </row>
-    <row r="32" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B32" s="21">
         <v>27</v>
       </c>
@@ -5672,7 +5674,7 @@
       <c r="BO32" s="2"/>
       <c r="BP32" s="2"/>
     </row>
-    <row r="33" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B33" s="21">
         <v>28</v>
       </c>
@@ -5747,7 +5749,7 @@
       <c r="BO33" s="2"/>
       <c r="BP33" s="2"/>
     </row>
-    <row r="34" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B34" s="21">
         <v>29</v>
       </c>
@@ -5828,7 +5830,7 @@
       <c r="BO34" s="2"/>
       <c r="BP34" s="2"/>
     </row>
-    <row r="35" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B35" s="21">
         <v>30</v>
       </c>
@@ -5905,7 +5907,7 @@
       <c r="BO35" s="2"/>
       <c r="BP35" s="2"/>
     </row>
-    <row r="36" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B36" s="21">
         <v>31</v>
       </c>
@@ -5982,7 +5984,7 @@
       <c r="BO36" s="2"/>
       <c r="BP36" s="2"/>
     </row>
-    <row r="37" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B37" s="22">
         <v>32</v>
       </c>
@@ -6059,7 +6061,7 @@
       <c r="BO37" s="4"/>
       <c r="BP37" s="4"/>
     </row>
-    <row r="38" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B38" s="23">
         <v>33</v>
       </c>
@@ -6134,7 +6136,7 @@
       <c r="BO38" s="4"/>
       <c r="BP38" s="4"/>
     </row>
-    <row r="39" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B39" s="22">
         <v>34</v>
       </c>
@@ -6209,7 +6211,7 @@
       <c r="BO39" s="2"/>
       <c r="BP39" s="2"/>
     </row>
-    <row r="40" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B40" s="23">
         <v>35</v>
       </c>
@@ -6284,7 +6286,7 @@
       <c r="BO40" s="2"/>
       <c r="BP40" s="2"/>
     </row>
-    <row r="41" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B41" s="22">
         <v>36</v>
       </c>
@@ -6359,7 +6361,7 @@
       <c r="BO41" s="2"/>
       <c r="BP41" s="2"/>
     </row>
-    <row r="42" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B42" s="23">
         <v>37</v>
       </c>
@@ -6434,7 +6436,7 @@
       <c r="BO42" s="2"/>
       <c r="BP42" s="2"/>
     </row>
-    <row r="43" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B43" s="22">
         <v>38</v>
       </c>
@@ -6511,7 +6513,7 @@
       <c r="BO43" s="2"/>
       <c r="BP43" s="2"/>
     </row>
-    <row r="44" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B44" s="23">
         <v>39</v>
       </c>
@@ -6586,7 +6588,7 @@
       <c r="BO44" s="2"/>
       <c r="BP44" s="2"/>
     </row>
-    <row r="45" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B45" s="22">
         <v>40</v>
       </c>
@@ -6661,7 +6663,7 @@
       <c r="BO45" s="2"/>
       <c r="BP45" s="2"/>
     </row>
-    <row r="46" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B46" s="23">
         <v>41</v>
       </c>
@@ -6734,7 +6736,7 @@
       <c r="BO46" s="2"/>
       <c r="BP46" s="2"/>
     </row>
-    <row r="47" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B47" s="23">
         <v>42</v>
       </c>
@@ -6811,7 +6813,7 @@
       <c r="BO47" s="2"/>
       <c r="BP47" s="2"/>
     </row>
-    <row r="48" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B48" s="22">
         <v>43</v>
       </c>
@@ -6888,7 +6890,7 @@
       <c r="BO48" s="4"/>
       <c r="BP48" s="4"/>
     </row>
-    <row r="49" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B49" s="23">
         <v>44</v>
       </c>
@@ -6965,7 +6967,7 @@
       <c r="BO49" s="2"/>
       <c r="BP49" s="2"/>
     </row>
-    <row r="50" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B50" s="23">
         <v>45</v>
       </c>
@@ -7042,7 +7044,7 @@
       <c r="BO50" s="2"/>
       <c r="BP50" s="2"/>
     </row>
-    <row r="51" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B51" s="22">
         <v>46</v>
       </c>
@@ -7119,7 +7121,7 @@
       <c r="BO51" s="27"/>
       <c r="BP51" s="27"/>
     </row>
-    <row r="52" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B52" s="23">
         <v>47</v>
       </c>
@@ -7194,7 +7196,7 @@
       <c r="BO52" s="3"/>
       <c r="BP52" s="3"/>
     </row>
-    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B53" s="23">
         <v>48</v>
       </c>
@@ -7271,7 +7273,7 @@
       <c r="BO53" s="3"/>
       <c r="BP53" s="3"/>
     </row>
-    <row r="54" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B54" s="30" t="s">
         <v>69</v>
       </c>
@@ -7454,90 +7456,90 @@
       </c>
       <c r="AV54" s="5">
         <f t="shared" ref="AV54" si="24">AU54-SUM(AV6:AV53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="AW54" s="5">
         <f t="shared" ref="AW54" si="25">AV54-SUM(AW6:AW53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="AX54" s="5">
         <f t="shared" ref="AX54" si="26">AW54-SUM(AX6:AX53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="AY54" s="5">
         <f t="shared" ref="AY54" si="27">AX54-SUM(AY6:AY53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="AZ54" s="5">
         <f t="shared" ref="AZ54" si="28">AY54-SUM(AZ6:AZ53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BA54" s="5">
         <f t="shared" ref="BA54" si="29">AZ54-SUM(BA6:BA53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BB54" s="5">
         <f t="shared" ref="BB54" si="30">BA54-SUM(BB6:BB53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BC54" s="5">
         <f t="shared" ref="BC54" si="31">BB54-SUM(BC6:BC53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BD54" s="5">
         <f t="shared" ref="BD54" si="32">BC54-SUM(BD6:BD53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BE54" s="5">
         <f t="shared" ref="BE54" si="33">BD54-SUM(BE6:BE53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BF54" s="5">
         <f t="shared" ref="BF54" si="34">BE54-SUM(BF6:BF53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BG54" s="5">
         <f t="shared" ref="BG54" si="35">BF54-SUM(BG6:BG53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BH54" s="5">
         <f t="shared" ref="BH54" si="36">BG54-SUM(BH6:BH53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BI54" s="5">
         <f t="shared" ref="BI54" si="37">BH54-SUM(BI6:BI53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BJ54" s="5">
         <f t="shared" ref="BJ54:BL54" si="38">BI54-SUM(BJ6:BJ53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BK54" s="5">
         <f t="shared" si="38"/>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BL54" s="5">
         <f t="shared" si="38"/>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BM54" s="5">
         <f t="shared" ref="BM54" si="39">BL54-SUM(BM6:BM53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BN54" s="5">
         <f t="shared" ref="BN54" si="40">BM54-SUM(BN6:BN53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BO54" s="5">
         <f t="shared" ref="BO54" si="41">BN54-SUM(BO6:BO53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="BP54" s="5">
         <f>BO54-SUM(BP6:BP53)</f>
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
     </row>
-    <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B55" s="32" t="s">
         <v>70</v>
       </c>
@@ -7803,17 +7805,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B56" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B57" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="15" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
Boekingen fix, tocht select
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CD71BF-9B55-4EFB-B6C7-B51D1F9D56D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C230E1-5F1F-47BF-A8CD-2E2E72ABB091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
@@ -450,7 +450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +514,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -826,12 +838,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -874,6 +880,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1318,100 +1339,100 @@
                   <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>54</c:v>
-                </c:pt>
                 <c:pt idx="37">
-                  <c:v>49</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>49.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>46.5</c:v>
                 </c:pt>
-                <c:pt idx="40">
-                  <c:v>46.5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>45.5</c:v>
-                </c:pt>
                 <c:pt idx="42">
-                  <c:v>41.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>41.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>32.5</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>29.5</c:v>
-                </c:pt>
                 <c:pt idx="46">
-                  <c:v>29.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>29.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>29.5</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>29.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>29.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3030,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AW15" sqref="AW15:AX15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BA9" sqref="BA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3045,98 +3066,98 @@
   <sheetData>
     <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:69" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
-      <c r="AW2" s="34"/>
-      <c r="AX2" s="34"/>
-      <c r="AY2" s="34"/>
-      <c r="AZ2" s="34"/>
-      <c r="BA2" s="34"/>
-      <c r="BB2" s="34"/>
-      <c r="BC2" s="34"/>
-      <c r="BD2" s="34"/>
-      <c r="BE2" s="34"/>
-      <c r="BF2" s="34"/>
-      <c r="BG2" s="34"/>
-      <c r="BH2" s="34"/>
-      <c r="BI2" s="34"/>
-      <c r="BJ2" s="34"/>
-      <c r="BK2" s="34"/>
-      <c r="BL2" s="34"/>
-      <c r="BM2" s="34"/>
-      <c r="BN2" s="34"/>
-      <c r="BO2" s="34"/>
-      <c r="BP2" s="34"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="32"/>
+      <c r="BH2" s="32"/>
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="32"/>
+      <c r="BK2" s="32"/>
+      <c r="BL2" s="32"/>
+      <c r="BM2" s="32"/>
+      <c r="BN2" s="32"/>
+      <c r="BO2" s="32"/>
+      <c r="BP2" s="32"/>
       <c r="BQ2" s="1"/>
     </row>
     <row r="3" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -3186,10 +3207,10 @@
       <c r="BP3" s="3"/>
     </row>
     <row r="4" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
@@ -3389,8 +3410,8 @@
       </c>
     </row>
     <row r="5" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="18" t="s">
         <v>4</v>
       </c>
@@ -3863,23 +3884,27 @@
       <c r="AJ9" s="10">
         <v>1</v>
       </c>
-      <c r="AK9" s="2"/>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="2"/>
-      <c r="AQ9" s="2"/>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="2"/>
-      <c r="AT9" s="2"/>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="2"/>
-      <c r="AW9" s="2"/>
-      <c r="AX9" s="2"/>
-      <c r="AY9" s="2"/>
-      <c r="AZ9" s="2"/>
-      <c r="BA9" s="2"/>
+      <c r="AK9" s="12">
+        <v>-1</v>
+      </c>
+      <c r="AL9" s="12"/>
+      <c r="AM9" s="12"/>
+      <c r="AN9" s="12"/>
+      <c r="AO9" s="12"/>
+      <c r="AP9" s="12"/>
+      <c r="AQ9" s="12"/>
+      <c r="AR9" s="12"/>
+      <c r="AS9" s="12"/>
+      <c r="AT9" s="12"/>
+      <c r="AU9" s="12"/>
+      <c r="AV9" s="12"/>
+      <c r="AW9" s="12"/>
+      <c r="AX9" s="12"/>
+      <c r="AY9" s="12"/>
+      <c r="AZ9" s="12"/>
+      <c r="BA9" s="10">
+        <v>1</v>
+      </c>
       <c r="BB9" s="2"/>
       <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
@@ -3951,12 +3976,16 @@
       <c r="AU10" s="10">
         <v>1</v>
       </c>
-      <c r="AV10" s="2"/>
-      <c r="AW10" s="2"/>
-      <c r="AX10" s="2"/>
-      <c r="AY10" s="2"/>
-      <c r="AZ10" s="2"/>
-      <c r="BA10" s="2"/>
+      <c r="AV10" s="12">
+        <v>-1</v>
+      </c>
+      <c r="AW10" s="12"/>
+      <c r="AX10" s="12"/>
+      <c r="AY10" s="12"/>
+      <c r="AZ10" s="12"/>
+      <c r="BA10" s="10">
+        <v>1</v>
+      </c>
       <c r="BB10" s="2"/>
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
@@ -4457,25 +4486,25 @@
       <c r="D17" s="10">
         <v>2</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
       <c r="X17" s="12">
         <v>1</v>
       </c>
@@ -4579,17 +4608,19 @@
       <c r="AO18" s="10">
         <v>0.5</v>
       </c>
-      <c r="AP18" s="2"/>
-      <c r="AQ18" s="2"/>
-      <c r="AR18" s="2"/>
-      <c r="AS18" s="2"/>
-      <c r="AT18" s="2"/>
-      <c r="AU18" s="2"/>
-      <c r="AV18" s="2"/>
-      <c r="AW18" s="2"/>
-      <c r="AX18" s="2"/>
-      <c r="AY18" s="2"/>
-      <c r="AZ18" s="2"/>
+      <c r="AP18" s="12"/>
+      <c r="AQ18" s="12"/>
+      <c r="AR18" s="12"/>
+      <c r="AS18" s="12"/>
+      <c r="AT18" s="12"/>
+      <c r="AU18" s="12"/>
+      <c r="AV18" s="12"/>
+      <c r="AW18" s="12"/>
+      <c r="AX18" s="12"/>
+      <c r="AY18" s="12"/>
+      <c r="AZ18" s="12">
+        <v>-0.5</v>
+      </c>
       <c r="BA18" s="2"/>
       <c r="BB18" s="2"/>
       <c r="BC18" s="2"/>
@@ -4846,61 +4877,63 @@
       <c r="B22" s="21">
         <v>17</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="10">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-      <c r="Z22" s="2"/>
-      <c r="AA22" s="2"/>
-      <c r="AB22" s="2"/>
-      <c r="AC22" s="2"/>
-      <c r="AD22" s="2"/>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
-      <c r="AG22" s="2"/>
-      <c r="AH22" s="2"/>
-      <c r="AI22" s="2"/>
-      <c r="AJ22" s="2"/>
-      <c r="AK22" s="2"/>
-      <c r="AL22" s="2"/>
-      <c r="AM22" s="2"/>
-      <c r="AN22" s="2"/>
-      <c r="AO22" s="2"/>
-      <c r="AP22" s="2"/>
-      <c r="AQ22" s="2"/>
-      <c r="AR22" s="2"/>
-      <c r="AS22" s="2"/>
-      <c r="AT22" s="2"/>
-      <c r="AU22" s="2"/>
-      <c r="AV22" s="2"/>
-      <c r="AW22" s="2"/>
-      <c r="AX22" s="2"/>
-      <c r="AY22" s="2"/>
-      <c r="AZ22" s="2"/>
-      <c r="BA22" s="2"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="16"/>
+      <c r="AB22" s="16"/>
+      <c r="AC22" s="16"/>
+      <c r="AD22" s="16"/>
+      <c r="AE22" s="16"/>
+      <c r="AF22" s="16"/>
+      <c r="AG22" s="16"/>
+      <c r="AH22" s="16"/>
+      <c r="AI22" s="16"/>
+      <c r="AJ22" s="16"/>
+      <c r="AK22" s="16"/>
+      <c r="AL22" s="16"/>
+      <c r="AM22" s="16"/>
+      <c r="AN22" s="16"/>
+      <c r="AO22" s="16"/>
+      <c r="AP22" s="16"/>
+      <c r="AQ22" s="16"/>
+      <c r="AR22" s="16"/>
+      <c r="AS22" s="16"/>
+      <c r="AT22" s="16"/>
+      <c r="AU22" s="16"/>
+      <c r="AV22" s="16"/>
+      <c r="AW22" s="16"/>
+      <c r="AX22" s="16"/>
+      <c r="AY22" s="16"/>
+      <c r="AZ22" s="16"/>
+      <c r="BA22" s="10">
+        <v>2</v>
+      </c>
       <c r="BB22" s="2"/>
       <c r="BC22" s="2"/>
       <c r="BD22" s="2"/>
@@ -6065,7 +6098,7 @@
       <c r="B38" s="23">
         <v>33</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="43" t="s">
         <v>112</v>
       </c>
       <c r="D38" s="20">
@@ -6140,61 +6173,63 @@
       <c r="B39" s="22">
         <v>34</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D39" s="10">
         <v>1</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="2"/>
-      <c r="AI39" s="2"/>
-      <c r="AJ39" s="2"/>
-      <c r="AK39" s="2"/>
-      <c r="AL39" s="2"/>
-      <c r="AM39" s="2"/>
-      <c r="AN39" s="2"/>
-      <c r="AO39" s="2"/>
-      <c r="AP39" s="2"/>
-      <c r="AQ39" s="2"/>
-      <c r="AR39" s="2"/>
-      <c r="AS39" s="2"/>
-      <c r="AT39" s="2"/>
-      <c r="AU39" s="2"/>
-      <c r="AV39" s="2"/>
-      <c r="AW39" s="2"/>
-      <c r="AX39" s="2"/>
-      <c r="AY39" s="2"/>
-      <c r="AZ39" s="2"/>
-      <c r="BA39" s="2"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="16"/>
+      <c r="AB39" s="16"/>
+      <c r="AC39" s="16"/>
+      <c r="AD39" s="16"/>
+      <c r="AE39" s="16"/>
+      <c r="AF39" s="16"/>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="16"/>
+      <c r="AI39" s="16"/>
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="16"/>
+      <c r="AL39" s="16"/>
+      <c r="AM39" s="16"/>
+      <c r="AN39" s="16"/>
+      <c r="AO39" s="16"/>
+      <c r="AP39" s="16"/>
+      <c r="AQ39" s="16"/>
+      <c r="AR39" s="16"/>
+      <c r="AS39" s="16"/>
+      <c r="AT39" s="16"/>
+      <c r="AU39" s="16"/>
+      <c r="AV39" s="16"/>
+      <c r="AW39" s="16"/>
+      <c r="AX39" s="16"/>
+      <c r="AY39" s="16"/>
+      <c r="AZ39" s="16"/>
+      <c r="BA39" s="10">
+        <v>1</v>
+      </c>
       <c r="BB39" s="2"/>
       <c r="BC39" s="2"/>
       <c r="BD39" s="2"/>
@@ -6215,7 +6250,7 @@
       <c r="B40" s="23">
         <v>35</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="43" t="s">
         <v>114</v>
       </c>
       <c r="D40" s="20">
@@ -6290,10 +6325,10 @@
       <c r="B41" s="22">
         <v>36</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="27">
         <v>1</v>
       </c>
       <c r="E41" s="2"/>
@@ -6365,7 +6400,7 @@
       <c r="B42" s="23">
         <v>37</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="40" t="s">
         <v>116</v>
       </c>
       <c r="D42" s="20">
@@ -6440,7 +6475,7 @@
       <c r="B43" s="22">
         <v>38</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="26" t="s">
         <v>117</v>
       </c>
       <c r="D43" s="10">
@@ -6491,12 +6526,16 @@
       <c r="AU43" s="10">
         <v>1</v>
       </c>
-      <c r="AV43" s="2"/>
-      <c r="AW43" s="2"/>
-      <c r="AX43" s="2"/>
-      <c r="AY43" s="2"/>
-      <c r="AZ43" s="2"/>
-      <c r="BA43" s="2"/>
+      <c r="AV43" s="12">
+        <v>-1</v>
+      </c>
+      <c r="AW43" s="12"/>
+      <c r="AX43" s="12"/>
+      <c r="AY43" s="12"/>
+      <c r="AZ43" s="12"/>
+      <c r="BA43" s="10">
+        <v>1</v>
+      </c>
       <c r="BB43" s="2"/>
       <c r="BC43" s="2"/>
       <c r="BD43" s="2"/>
@@ -6517,7 +6556,7 @@
       <c r="B44" s="23">
         <v>39</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="41" t="s">
         <v>118</v>
       </c>
       <c r="D44" s="20">
@@ -6592,7 +6631,7 @@
       <c r="B45" s="22">
         <v>40</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="41" t="s">
         <v>119</v>
       </c>
       <c r="D45" s="20">
@@ -6667,8 +6706,8 @@
       <c r="B46" s="23">
         <v>41</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="29">
+      <c r="C46" s="42"/>
+      <c r="D46" s="27">
         <v>1</v>
       </c>
       <c r="E46" s="2"/>
@@ -7092,34 +7131,34 @@
       <c r="AL51" s="2"/>
       <c r="AM51" s="2"/>
       <c r="AN51" s="2"/>
-      <c r="AO51" s="27"/>
-      <c r="AP51" s="27"/>
-      <c r="AQ51" s="27"/>
-      <c r="AR51" s="27"/>
-      <c r="AS51" s="27"/>
-      <c r="AT51" s="27"/>
-      <c r="AU51" s="27"/>
-      <c r="AV51" s="27"/>
-      <c r="AW51" s="27"/>
-      <c r="AX51" s="27"/>
-      <c r="AY51" s="27"/>
-      <c r="AZ51" s="27"/>
-      <c r="BA51" s="27"/>
-      <c r="BB51" s="27"/>
-      <c r="BC51" s="27"/>
-      <c r="BD51" s="27"/>
-      <c r="BE51" s="27"/>
-      <c r="BF51" s="27"/>
-      <c r="BG51" s="27"/>
-      <c r="BH51" s="27"/>
-      <c r="BI51" s="27"/>
-      <c r="BJ51" s="27"/>
-      <c r="BK51" s="27"/>
-      <c r="BL51" s="27"/>
-      <c r="BM51" s="27"/>
-      <c r="BN51" s="27"/>
-      <c r="BO51" s="27"/>
-      <c r="BP51" s="27"/>
+      <c r="AO51" s="25"/>
+      <c r="AP51" s="25"/>
+      <c r="AQ51" s="25"/>
+      <c r="AR51" s="25"/>
+      <c r="AS51" s="25"/>
+      <c r="AT51" s="25"/>
+      <c r="AU51" s="25"/>
+      <c r="AV51" s="25"/>
+      <c r="AW51" s="25"/>
+      <c r="AX51" s="25"/>
+      <c r="AY51" s="25"/>
+      <c r="AZ51" s="25"/>
+      <c r="BA51" s="25"/>
+      <c r="BB51" s="25"/>
+      <c r="BC51" s="25"/>
+      <c r="BD51" s="25"/>
+      <c r="BE51" s="25"/>
+      <c r="BF51" s="25"/>
+      <c r="BG51" s="25"/>
+      <c r="BH51" s="25"/>
+      <c r="BI51" s="25"/>
+      <c r="BJ51" s="25"/>
+      <c r="BK51" s="25"/>
+      <c r="BL51" s="25"/>
+      <c r="BM51" s="25"/>
+      <c r="BN51" s="25"/>
+      <c r="BO51" s="25"/>
+      <c r="BP51" s="25"/>
     </row>
     <row r="52" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B52" s="23">
@@ -7274,10 +7313,10 @@
       <c r="BP53" s="3"/>
     </row>
     <row r="54" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="31"/>
+      <c r="C54" s="29"/>
       <c r="D54" s="24">
         <f>SUM(D6:D53)</f>
         <v>64</v>
@@ -7412,138 +7451,138 @@
       </c>
       <c r="AK54" s="5">
         <f t="shared" ref="AK54" si="15">AJ54-SUM(AK6:AK53)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AL54" s="5">
         <f t="shared" ref="AL54" si="16">AK54-SUM(AL6:AL53)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AM54" s="5">
         <f>AL54-SUM(AM6:AM53)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AN54" s="5">
         <f t="shared" ref="AN54" si="17">AM54-SUM(AN6:AN53)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AO54" s="5">
         <f>AN54-SUM(AO6:AO53)</f>
-        <v>49.5</v>
+        <v>50.5</v>
       </c>
       <c r="AP54" s="5">
         <f t="shared" ref="AP54" si="18">AO54-SUM(AP6:AP53)</f>
-        <v>46.5</v>
+        <v>47.5</v>
       </c>
       <c r="AQ54" s="5">
         <f t="shared" ref="AQ54" si="19">AP54-SUM(AQ6:AQ53)</f>
-        <v>46.5</v>
+        <v>47.5</v>
       </c>
       <c r="AR54" s="5">
         <f t="shared" ref="AR54" si="20">AQ54-SUM(AR6:AR53)</f>
-        <v>45.5</v>
+        <v>46.5</v>
       </c>
       <c r="AS54" s="5">
         <f t="shared" ref="AS54" si="21">AR54-SUM(AS6:AS53)</f>
-        <v>41.5</v>
+        <v>42.5</v>
       </c>
       <c r="AT54" s="5">
         <f t="shared" ref="AT54" si="22">AS54-SUM(AT6:AT53)</f>
-        <v>41.5</v>
+        <v>42.5</v>
       </c>
       <c r="AU54" s="5">
         <f t="shared" ref="AU54" si="23">AT54-SUM(AU6:AU53)</f>
-        <v>32.5</v>
+        <v>33.5</v>
       </c>
       <c r="AV54" s="5">
         <f t="shared" ref="AV54" si="24">AU54-SUM(AV6:AV53)</f>
-        <v>29.5</v>
+        <v>32.5</v>
       </c>
       <c r="AW54" s="5">
         <f t="shared" ref="AW54" si="25">AV54-SUM(AW6:AW53)</f>
-        <v>29.5</v>
+        <v>32.5</v>
       </c>
       <c r="AX54" s="5">
         <f t="shared" ref="AX54" si="26">AW54-SUM(AX6:AX53)</f>
-        <v>29.5</v>
+        <v>32.5</v>
       </c>
       <c r="AY54" s="5">
         <f t="shared" ref="AY54" si="27">AX54-SUM(AY6:AY53)</f>
-        <v>29.5</v>
+        <v>32.5</v>
       </c>
       <c r="AZ54" s="5">
         <f t="shared" ref="AZ54" si="28">AY54-SUM(AZ6:AZ53)</f>
-        <v>29.5</v>
+        <v>33</v>
       </c>
       <c r="BA54" s="5">
         <f t="shared" ref="BA54" si="29">AZ54-SUM(BA6:BA53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BB54" s="5">
         <f t="shared" ref="BB54" si="30">BA54-SUM(BB6:BB53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BC54" s="5">
         <f t="shared" ref="BC54" si="31">BB54-SUM(BC6:BC53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BD54" s="5">
         <f t="shared" ref="BD54" si="32">BC54-SUM(BD6:BD53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BE54" s="5">
         <f t="shared" ref="BE54" si="33">BD54-SUM(BE6:BE53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BF54" s="5">
         <f t="shared" ref="BF54" si="34">BE54-SUM(BF6:BF53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BG54" s="5">
         <f t="shared" ref="BG54" si="35">BF54-SUM(BG6:BG53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BH54" s="5">
         <f t="shared" ref="BH54" si="36">BG54-SUM(BH6:BH53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BI54" s="5">
         <f t="shared" ref="BI54" si="37">BH54-SUM(BI6:BI53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BJ54" s="5">
         <f t="shared" ref="BJ54:BL54" si="38">BI54-SUM(BJ6:BJ53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BK54" s="5">
         <f t="shared" si="38"/>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BL54" s="5">
         <f t="shared" si="38"/>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BM54" s="5">
         <f t="shared" ref="BM54" si="39">BL54-SUM(BM6:BM53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BN54" s="5">
         <f t="shared" ref="BN54" si="40">BM54-SUM(BN6:BN53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BO54" s="5">
         <f t="shared" ref="BO54" si="41">BN54-SUM(BO6:BO53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
       <c r="BP54" s="5">
         <f>BO54-SUM(BP6:BP53)</f>
-        <v>29.5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="32" t="s">
+      <c r="B55" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="33"/>
+      <c r="C55" s="31"/>
       <c r="D55" s="6">
         <f>SUM(D6:D53)</f>
         <v>64</v>

</xml_diff>

<commit_message>
klant omgeving navbar bijgewerkt
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C230E1-5F1F-47BF-A8CD-2E2E72ABB091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FF66C0-CD64-41BE-B235-3B4C548A9C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -845,6 +845,21 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -880,21 +895,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1390,22 +1390,22 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>27</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>27</c:v>
@@ -3051,113 +3051,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BA9" sqref="BA9"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="BI9" sqref="BI9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" customWidth="1"/>
-    <col min="39" max="40" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="39" max="40" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:69" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="36" t="s">
+    <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:69" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-      <c r="AY2" s="32"/>
-      <c r="AZ2" s="32"/>
-      <c r="BA2" s="32"/>
-      <c r="BB2" s="32"/>
-      <c r="BC2" s="32"/>
-      <c r="BD2" s="32"/>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="32"/>
-      <c r="BG2" s="32"/>
-      <c r="BH2" s="32"/>
-      <c r="BI2" s="32"/>
-      <c r="BJ2" s="32"/>
-      <c r="BK2" s="32"/>
-      <c r="BL2" s="32"/>
-      <c r="BM2" s="32"/>
-      <c r="BN2" s="32"/>
-      <c r="BO2" s="32"/>
-      <c r="BP2" s="32"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="37"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="37"/>
+      <c r="BK2" s="37"/>
+      <c r="BL2" s="37"/>
+      <c r="BM2" s="37"/>
+      <c r="BN2" s="37"/>
+      <c r="BO2" s="37"/>
+      <c r="BP2" s="37"/>
       <c r="BQ2" s="1"/>
     </row>
-    <row r="3" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
+    <row r="3" spans="2:69" x14ac:dyDescent="0.3">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -3206,11 +3206,11 @@
       <c r="BO3" s="3"/>
       <c r="BP3" s="3"/>
     </row>
-    <row r="4" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="2:69" x14ac:dyDescent="0.3">
+      <c r="B4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="18" t="s">
@@ -3409,9 +3409,9 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="18" t="s">
         <v>4</v>
       </c>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="BQ5" s="1"/>
     </row>
-    <row r="6" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B6" s="21">
         <v>1</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="BO6" s="2"/>
       <c r="BP6" s="2"/>
     </row>
-    <row r="7" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B7" s="21">
         <v>2</v>
       </c>
@@ -3763,7 +3763,7 @@
       <c r="BO7" s="2"/>
       <c r="BP7" s="2"/>
     </row>
-    <row r="8" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B8" s="21">
         <v>3</v>
       </c>
@@ -3840,7 +3840,7 @@
       <c r="BO8" s="2"/>
       <c r="BP8" s="2"/>
     </row>
-    <row r="9" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B9" s="21">
         <v>4</v>
       </c>
@@ -3905,13 +3905,17 @@
       <c r="BA9" s="10">
         <v>1</v>
       </c>
-      <c r="BB9" s="2"/>
-      <c r="BC9" s="2"/>
-      <c r="BD9" s="2"/>
-      <c r="BE9" s="2"/>
-      <c r="BF9" s="2"/>
-      <c r="BG9" s="2"/>
-      <c r="BH9" s="2"/>
+      <c r="BB9" s="12">
+        <v>-0.5</v>
+      </c>
+      <c r="BC9" s="12"/>
+      <c r="BD9" s="12"/>
+      <c r="BE9" s="12"/>
+      <c r="BF9" s="12"/>
+      <c r="BG9" s="12"/>
+      <c r="BH9" s="10">
+        <v>0.5</v>
+      </c>
       <c r="BI9" s="2"/>
       <c r="BJ9" s="2"/>
       <c r="BK9" s="2"/>
@@ -3921,7 +3925,7 @@
       <c r="BO9" s="2"/>
       <c r="BP9" s="2"/>
     </row>
-    <row r="10" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B10" s="21">
         <v>5</v>
       </c>
@@ -4002,7 +4006,7 @@
       <c r="BO10" s="2"/>
       <c r="BP10" s="2"/>
     </row>
-    <row r="11" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B11" s="21">
         <v>6</v>
       </c>
@@ -4079,7 +4083,7 @@
       <c r="BO11" s="2"/>
       <c r="BP11" s="2"/>
     </row>
-    <row r="12" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B12" s="21">
         <v>7</v>
       </c>
@@ -4168,7 +4172,7 @@
       <c r="BO12" s="2"/>
       <c r="BP12" s="2"/>
     </row>
-    <row r="13" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B13" s="21">
         <v>8</v>
       </c>
@@ -4247,7 +4251,7 @@
       <c r="BO13" s="2"/>
       <c r="BP13" s="2"/>
     </row>
-    <row r="14" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B14" s="21">
         <v>9</v>
       </c>
@@ -4324,7 +4328,7 @@
       <c r="BO14" s="2"/>
       <c r="BP14" s="2"/>
     </row>
-    <row r="15" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B15" s="21">
         <v>10</v>
       </c>
@@ -4401,7 +4405,7 @@
       <c r="BO15" s="2"/>
       <c r="BP15" s="2"/>
     </row>
-    <row r="16" spans="2:69" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:69" x14ac:dyDescent="0.3">
       <c r="B16" s="21">
         <v>11</v>
       </c>
@@ -4476,7 +4480,7 @@
       <c r="BO16" s="2"/>
       <c r="BP16" s="2"/>
     </row>
-    <row r="17" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B17" s="21">
         <v>12</v>
       </c>
@@ -4559,7 +4563,7 @@
       <c r="BO17" s="2"/>
       <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B18" s="21">
         <v>13</v>
       </c>
@@ -4638,7 +4642,7 @@
       <c r="BO18" s="2"/>
       <c r="BP18" s="2"/>
     </row>
-    <row r="19" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B19" s="21">
         <v>14</v>
       </c>
@@ -4719,7 +4723,7 @@
       <c r="BO19" s="2"/>
       <c r="BP19" s="2"/>
     </row>
-    <row r="20" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B20" s="21">
         <v>15</v>
       </c>
@@ -4796,7 +4800,7 @@
       <c r="BO20" s="2"/>
       <c r="BP20" s="2"/>
     </row>
-    <row r="21" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B21" s="21">
         <v>16</v>
       </c>
@@ -4873,7 +4877,7 @@
       <c r="BO21" s="2"/>
       <c r="BP21" s="2"/>
     </row>
-    <row r="22" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B22" s="21">
         <v>17</v>
       </c>
@@ -4950,7 +4954,7 @@
       <c r="BO22" s="2"/>
       <c r="BP22" s="2"/>
     </row>
-    <row r="23" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B23" s="21">
         <v>18</v>
       </c>
@@ -5025,7 +5029,7 @@
       <c r="BO23" s="2"/>
       <c r="BP23" s="2"/>
     </row>
-    <row r="24" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B24" s="21">
         <v>19</v>
       </c>
@@ -5100,7 +5104,7 @@
       <c r="BO24" s="2"/>
       <c r="BP24" s="2"/>
     </row>
-    <row r="25" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B25" s="21">
         <v>20</v>
       </c>
@@ -5179,7 +5183,7 @@
       <c r="BO25" s="2"/>
       <c r="BP25" s="2"/>
     </row>
-    <row r="26" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B26" s="21">
         <v>21</v>
       </c>
@@ -5254,7 +5258,7 @@
       <c r="BO26" s="2"/>
       <c r="BP26" s="2"/>
     </row>
-    <row r="27" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B27" s="21">
         <v>22</v>
       </c>
@@ -5331,7 +5335,7 @@
       <c r="BO27" s="2"/>
       <c r="BP27" s="2"/>
     </row>
-    <row r="28" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B28" s="21">
         <v>23</v>
       </c>
@@ -5406,7 +5410,7 @@
       <c r="BO28" s="2"/>
       <c r="BP28" s="2"/>
     </row>
-    <row r="29" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B29" s="21">
         <v>24</v>
       </c>
@@ -5481,7 +5485,7 @@
       <c r="BO29" s="2"/>
       <c r="BP29" s="2"/>
     </row>
-    <row r="30" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B30" s="21">
         <v>25</v>
       </c>
@@ -5556,7 +5560,7 @@
       <c r="BO30" s="2"/>
       <c r="BP30" s="2"/>
     </row>
-    <row r="31" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B31" s="21">
         <v>26</v>
       </c>
@@ -5633,7 +5637,7 @@
       <c r="BO31" s="2"/>
       <c r="BP31" s="2"/>
     </row>
-    <row r="32" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B32" s="21">
         <v>27</v>
       </c>
@@ -5707,7 +5711,7 @@
       <c r="BO32" s="2"/>
       <c r="BP32" s="2"/>
     </row>
-    <row r="33" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B33" s="21">
         <v>28</v>
       </c>
@@ -5782,7 +5786,7 @@
       <c r="BO33" s="2"/>
       <c r="BP33" s="2"/>
     </row>
-    <row r="34" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B34" s="21">
         <v>29</v>
       </c>
@@ -5863,7 +5867,7 @@
       <c r="BO34" s="2"/>
       <c r="BP34" s="2"/>
     </row>
-    <row r="35" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B35" s="21">
         <v>30</v>
       </c>
@@ -5940,7 +5944,7 @@
       <c r="BO35" s="2"/>
       <c r="BP35" s="2"/>
     </row>
-    <row r="36" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B36" s="21">
         <v>31</v>
       </c>
@@ -6017,7 +6021,7 @@
       <c r="BO36" s="2"/>
       <c r="BP36" s="2"/>
     </row>
-    <row r="37" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B37" s="22">
         <v>32</v>
       </c>
@@ -6094,11 +6098,11 @@
       <c r="BO37" s="4"/>
       <c r="BP37" s="4"/>
     </row>
-    <row r="38" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B38" s="23">
         <v>33</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="31" t="s">
         <v>112</v>
       </c>
       <c r="D38" s="20">
@@ -6169,7 +6173,7 @@
       <c r="BO38" s="4"/>
       <c r="BP38" s="4"/>
     </row>
-    <row r="39" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B39" s="22">
         <v>34</v>
       </c>
@@ -6246,11 +6250,11 @@
       <c r="BO39" s="2"/>
       <c r="BP39" s="2"/>
     </row>
-    <row r="40" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B40" s="23">
         <v>35</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="31" t="s">
         <v>114</v>
       </c>
       <c r="D40" s="20">
@@ -6321,11 +6325,11 @@
       <c r="BO40" s="2"/>
       <c r="BP40" s="2"/>
     </row>
-    <row r="41" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B41" s="22">
         <v>36</v>
       </c>
-      <c r="C41" s="44" t="s">
+      <c r="C41" s="32" t="s">
         <v>115</v>
       </c>
       <c r="D41" s="27">
@@ -6396,11 +6400,11 @@
       <c r="BO41" s="2"/>
       <c r="BP41" s="2"/>
     </row>
-    <row r="42" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B42" s="23">
         <v>37</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="28" t="s">
         <v>116</v>
       </c>
       <c r="D42" s="20">
@@ -6471,7 +6475,7 @@
       <c r="BO42" s="2"/>
       <c r="BP42" s="2"/>
     </row>
-    <row r="43" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B43" s="22">
         <v>38</v>
       </c>
@@ -6552,11 +6556,11 @@
       <c r="BO43" s="2"/>
       <c r="BP43" s="2"/>
     </row>
-    <row r="44" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B44" s="23">
         <v>39</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="29" t="s">
         <v>118</v>
       </c>
       <c r="D44" s="20">
@@ -6627,11 +6631,11 @@
       <c r="BO44" s="2"/>
       <c r="BP44" s="2"/>
     </row>
-    <row r="45" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B45" s="22">
         <v>40</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="29" t="s">
         <v>119</v>
       </c>
       <c r="D45" s="20">
@@ -6702,11 +6706,11 @@
       <c r="BO45" s="2"/>
       <c r="BP45" s="2"/>
     </row>
-    <row r="46" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B46" s="23">
         <v>41</v>
       </c>
-      <c r="C46" s="42"/>
+      <c r="C46" s="30"/>
       <c r="D46" s="27">
         <v>1</v>
       </c>
@@ -6775,7 +6779,7 @@
       <c r="BO46" s="2"/>
       <c r="BP46" s="2"/>
     </row>
-    <row r="47" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B47" s="23">
         <v>42</v>
       </c>
@@ -6852,7 +6856,7 @@
       <c r="BO47" s="2"/>
       <c r="BP47" s="2"/>
     </row>
-    <row r="48" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B48" s="22">
         <v>43</v>
       </c>
@@ -6929,7 +6933,7 @@
       <c r="BO48" s="4"/>
       <c r="BP48" s="4"/>
     </row>
-    <row r="49" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B49" s="23">
         <v>44</v>
       </c>
@@ -7006,7 +7010,7 @@
       <c r="BO49" s="2"/>
       <c r="BP49" s="2"/>
     </row>
-    <row r="50" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B50" s="23">
         <v>45</v>
       </c>
@@ -7083,7 +7087,7 @@
       <c r="BO50" s="2"/>
       <c r="BP50" s="2"/>
     </row>
-    <row r="51" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B51" s="22">
         <v>46</v>
       </c>
@@ -7160,7 +7164,7 @@
       <c r="BO51" s="25"/>
       <c r="BP51" s="25"/>
     </row>
-    <row r="52" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B52" s="23">
         <v>47</v>
       </c>
@@ -7235,7 +7239,7 @@
       <c r="BO52" s="3"/>
       <c r="BP52" s="3"/>
     </row>
-    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="23">
         <v>48</v>
       </c>
@@ -7312,11 +7316,11 @@
       <c r="BO53" s="3"/>
       <c r="BP53" s="3"/>
     </row>
-    <row r="54" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B54" s="28" t="s">
+    <row r="54" spans="2:68" x14ac:dyDescent="0.3">
+      <c r="B54" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="29"/>
+      <c r="C54" s="34"/>
       <c r="D54" s="24">
         <f>SUM(D6:D53)</f>
         <v>64</v>
@@ -7519,27 +7523,27 @@
       </c>
       <c r="BB54" s="5">
         <f t="shared" ref="BB54" si="30">BA54-SUM(BB6:BB53)</f>
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="BC54" s="5">
         <f t="shared" ref="BC54" si="31">BB54-SUM(BC6:BC53)</f>
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="BD54" s="5">
         <f t="shared" ref="BD54" si="32">BC54-SUM(BD6:BD53)</f>
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="BE54" s="5">
         <f t="shared" ref="BE54" si="33">BD54-SUM(BE6:BE53)</f>
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="BF54" s="5">
         <f t="shared" ref="BF54" si="34">BE54-SUM(BF6:BF53)</f>
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="BG54" s="5">
         <f t="shared" ref="BG54" si="35">BF54-SUM(BG6:BG53)</f>
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="BH54" s="5">
         <f t="shared" ref="BH54" si="36">BG54-SUM(BH6:BH53)</f>
@@ -7578,11 +7582,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="30" t="s">
+    <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="31"/>
+      <c r="C55" s="36"/>
       <c r="D55" s="6">
         <f>SUM(D6:D53)</f>
         <v>64</v>
@@ -7844,17 +7848,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B56" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="2:68" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:68" x14ac:dyDescent="0.3">
       <c r="B57" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B58" s="15" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
client_klant_nav pin button, route text added
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37999DE4-F338-403E-B8D8-07837B44FF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0657A54-4E39-46B4-87A1-D79643F745D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
@@ -761,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -839,6 +839,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -875,12 +878,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -889,8 +886,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FF99FF99"/>
-      <color rgb="FFCCFFCC"/>
       <color rgb="FF33CC33"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFF0066"/>
@@ -1321,7 +1318,7 @@
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>56</c:v>
+                  <c:v>56.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>56</c:v>
@@ -1372,28 +1369,28 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>27</c:v>
+                  <c:v>26.9</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>27.5</c:v>
+                  <c:v>27.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>27.5</c:v>
+                  <c:v>27.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>27.5</c:v>
+                  <c:v>27.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>27.5</c:v>
+                  <c:v>27.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>27.5</c:v>
+                  <c:v>27.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>27.5</c:v>
+                  <c:v>27.099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>27</c:v>
+                  <c:v>26.9</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>23.5</c:v>
@@ -1402,22 +1399,22 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>17</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>17</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>17</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>17</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>17</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>17</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3036,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="BJ41" sqref="BJ41"/>
+    <sheetView tabSelected="1" topLeftCell="AR9" workbookViewId="0">
+      <selection activeCell="AY18" sqref="AP18:AY18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3051,98 +3048,98 @@
   <sheetData>
     <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:69" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
-      <c r="AV2" s="33"/>
-      <c r="AW2" s="33"/>
-      <c r="AX2" s="33"/>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="33"/>
-      <c r="BH2" s="33"/>
-      <c r="BI2" s="33"/>
-      <c r="BJ2" s="33"/>
-      <c r="BK2" s="33"/>
-      <c r="BL2" s="33"/>
-      <c r="BM2" s="33"/>
-      <c r="BN2" s="33"/>
-      <c r="BO2" s="33"/>
-      <c r="BP2" s="33"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+      <c r="AL2" s="34"/>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="34"/>
+      <c r="AT2" s="34"/>
+      <c r="AU2" s="34"/>
+      <c r="AV2" s="34"/>
+      <c r="AW2" s="34"/>
+      <c r="AX2" s="34"/>
+      <c r="AY2" s="34"/>
+      <c r="AZ2" s="34"/>
+      <c r="BA2" s="34"/>
+      <c r="BB2" s="34"/>
+      <c r="BC2" s="34"/>
+      <c r="BD2" s="34"/>
+      <c r="BE2" s="34"/>
+      <c r="BF2" s="34"/>
+      <c r="BG2" s="34"/>
+      <c r="BH2" s="34"/>
+      <c r="BI2" s="34"/>
+      <c r="BJ2" s="34"/>
+      <c r="BK2" s="34"/>
+      <c r="BL2" s="34"/>
+      <c r="BM2" s="34"/>
+      <c r="BN2" s="34"/>
+      <c r="BO2" s="34"/>
+      <c r="BP2" s="34"/>
       <c r="BQ2" s="1"/>
     </row>
     <row r="3" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="40"/>
-      <c r="S3" s="40"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -3192,10 +3189,10 @@
       <c r="BP3" s="3"/>
     </row>
     <row r="4" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="36" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
@@ -3395,8 +3392,8 @@
       </c>
     </row>
     <row r="5" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="17" t="s">
         <v>4</v>
       </c>
@@ -3867,44 +3864,48 @@
       <c r="AH9" s="15"/>
       <c r="AI9" s="15"/>
       <c r="AJ9" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK9" s="11">
-        <v>-1</v>
-      </c>
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="11"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
-      <c r="AP9" s="11"/>
-      <c r="AQ9" s="11"/>
-      <c r="AR9" s="11"/>
-      <c r="AS9" s="11"/>
-      <c r="AT9" s="11"/>
-      <c r="AU9" s="11"/>
-      <c r="AV9" s="11"/>
-      <c r="AW9" s="11"/>
-      <c r="AX9" s="11"/>
-      <c r="AY9" s="11"/>
-      <c r="AZ9" s="11"/>
+        <v>-0.5</v>
+      </c>
+      <c r="AL9" s="15"/>
+      <c r="AM9" s="15"/>
+      <c r="AN9" s="15"/>
+      <c r="AO9" s="15"/>
+      <c r="AP9" s="15"/>
+      <c r="AQ9" s="15"/>
+      <c r="AR9" s="15"/>
+      <c r="AS9" s="15"/>
+      <c r="AT9" s="15"/>
+      <c r="AU9" s="15"/>
+      <c r="AV9" s="15"/>
+      <c r="AW9" s="15"/>
+      <c r="AX9" s="15"/>
+      <c r="AY9" s="15"/>
+      <c r="AZ9" s="15"/>
       <c r="BA9" s="9">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="BB9" s="11">
-        <v>-0.5</v>
-      </c>
-      <c r="BC9" s="11"/>
-      <c r="BD9" s="11"/>
-      <c r="BE9" s="11"/>
-      <c r="BF9" s="11"/>
-      <c r="BG9" s="11"/>
+        <v>-0.2</v>
+      </c>
+      <c r="BC9" s="15"/>
+      <c r="BD9" s="15"/>
+      <c r="BE9" s="15"/>
+      <c r="BF9" s="15"/>
+      <c r="BG9" s="15"/>
       <c r="BH9" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="BI9" s="2"/>
-      <c r="BJ9" s="2"/>
-      <c r="BK9" s="2"/>
-      <c r="BL9" s="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="BI9" s="11">
+        <v>-0.1</v>
+      </c>
+      <c r="BJ9" s="15"/>
+      <c r="BK9" s="15"/>
+      <c r="BL9" s="9">
+        <v>0.1</v>
+      </c>
       <c r="BM9" s="2"/>
       <c r="BN9" s="2"/>
       <c r="BO9" s="2"/>
@@ -3968,10 +3969,10 @@
       <c r="AV10" s="11">
         <v>-1</v>
       </c>
-      <c r="AW10" s="11"/>
-      <c r="AX10" s="11"/>
-      <c r="AY10" s="11"/>
-      <c r="AZ10" s="11"/>
+      <c r="AW10" s="15"/>
+      <c r="AX10" s="15"/>
+      <c r="AY10" s="15"/>
+      <c r="AZ10" s="15"/>
       <c r="BA10" s="9">
         <v>1</v>
       </c>
@@ -4599,20 +4600,22 @@
       <c r="AO18" s="9">
         <v>0.5</v>
       </c>
-      <c r="AP18" s="11"/>
-      <c r="AQ18" s="11"/>
-      <c r="AR18" s="11"/>
-      <c r="AS18" s="11"/>
-      <c r="AT18" s="11"/>
-      <c r="AU18" s="11"/>
-      <c r="AV18" s="11"/>
-      <c r="AW18" s="11"/>
-      <c r="AX18" s="11"/>
-      <c r="AY18" s="11"/>
+      <c r="AP18" s="15"/>
+      <c r="AQ18" s="15"/>
+      <c r="AR18" s="15"/>
+      <c r="AS18" s="15"/>
+      <c r="AT18" s="15"/>
+      <c r="AU18" s="15"/>
+      <c r="AV18" s="15"/>
+      <c r="AW18" s="15"/>
+      <c r="AX18" s="15"/>
+      <c r="AY18" s="15"/>
       <c r="AZ18" s="11">
         <v>-0.5</v>
       </c>
-      <c r="BA18" s="2"/>
+      <c r="BA18" s="9">
+        <v>0.5</v>
+      </c>
       <c r="BB18" s="2"/>
       <c r="BC18" s="2"/>
       <c r="BD18" s="2"/>
@@ -5020,71 +5023,73 @@
       <c r="B24" s="20">
         <v>19</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="9">
         <v>2</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
-      <c r="Y24" s="2"/>
-      <c r="Z24" s="2"/>
-      <c r="AA24" s="2"/>
-      <c r="AB24" s="2"/>
-      <c r="AC24" s="2"/>
-      <c r="AD24" s="2"/>
-      <c r="AE24" s="2"/>
-      <c r="AF24" s="2"/>
-      <c r="AG24" s="2"/>
-      <c r="AH24" s="2"/>
-      <c r="AI24" s="2"/>
-      <c r="AJ24" s="2"/>
-      <c r="AK24" s="2"/>
-      <c r="AL24" s="2"/>
-      <c r="AM24" s="2"/>
-      <c r="AN24" s="2"/>
-      <c r="AO24" s="2"/>
-      <c r="AP24" s="2"/>
-      <c r="AQ24" s="2"/>
-      <c r="AR24" s="2"/>
-      <c r="AS24" s="2"/>
-      <c r="AT24" s="2"/>
-      <c r="AU24" s="2"/>
-      <c r="AV24" s="2"/>
-      <c r="AW24" s="2"/>
-      <c r="AX24" s="2"/>
-      <c r="AY24" s="2"/>
-      <c r="AZ24" s="2"/>
-      <c r="BA24" s="2"/>
-      <c r="BB24" s="2"/>
-      <c r="BC24" s="2"/>
-      <c r="BD24" s="2"/>
-      <c r="BE24" s="2"/>
-      <c r="BF24" s="2"/>
-      <c r="BG24" s="2"/>
-      <c r="BH24" s="2"/>
-      <c r="BI24" s="2"/>
-      <c r="BJ24" s="2"/>
-      <c r="BK24" s="2"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
+      <c r="AQ24" s="15"/>
+      <c r="AR24" s="15"/>
+      <c r="AS24" s="15"/>
+      <c r="AT24" s="15"/>
+      <c r="AU24" s="15"/>
+      <c r="AV24" s="15"/>
+      <c r="AW24" s="15"/>
+      <c r="AX24" s="15"/>
+      <c r="AY24" s="15"/>
+      <c r="AZ24" s="15"/>
+      <c r="BA24" s="15"/>
+      <c r="BB24" s="15"/>
+      <c r="BC24" s="15"/>
+      <c r="BD24" s="15"/>
+      <c r="BE24" s="15"/>
+      <c r="BF24" s="15"/>
+      <c r="BG24" s="15"/>
+      <c r="BH24" s="15"/>
+      <c r="BI24" s="15"/>
+      <c r="BJ24" s="15"/>
+      <c r="BK24" s="9">
+        <v>2</v>
+      </c>
       <c r="BL24" s="2"/>
       <c r="BM24" s="2"/>
       <c r="BN24" s="2"/>
@@ -6407,73 +6412,75 @@
       <c r="B42" s="22">
         <v>37</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="D42" s="42">
+      <c r="D42" s="10">
         <v>1</v>
       </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="11"/>
-      <c r="V42" s="11"/>
-      <c r="W42" s="11"/>
-      <c r="X42" s="11"/>
-      <c r="Y42" s="11"/>
-      <c r="Z42" s="11"/>
-      <c r="AA42" s="11"/>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="11"/>
-      <c r="AD42" s="11"/>
-      <c r="AE42" s="11"/>
-      <c r="AF42" s="11"/>
-      <c r="AG42" s="11"/>
-      <c r="AH42" s="11"/>
-      <c r="AI42" s="11"/>
-      <c r="AJ42" s="11"/>
-      <c r="AK42" s="11"/>
-      <c r="AL42" s="11"/>
-      <c r="AM42" s="11"/>
-      <c r="AN42" s="11"/>
-      <c r="AO42" s="11"/>
-      <c r="AP42" s="11"/>
-      <c r="AQ42" s="11"/>
-      <c r="AR42" s="11"/>
-      <c r="AS42" s="11"/>
-      <c r="AT42" s="11"/>
-      <c r="AU42" s="11"/>
-      <c r="AV42" s="11"/>
-      <c r="AW42" s="11"/>
-      <c r="AX42" s="11"/>
-      <c r="AY42" s="11"/>
-      <c r="AZ42" s="11"/>
-      <c r="BA42" s="11"/>
-      <c r="BB42" s="11"/>
-      <c r="BC42" s="11"/>
-      <c r="BD42" s="11"/>
-      <c r="BE42" s="11"/>
-      <c r="BF42" s="11"/>
-      <c r="BG42" s="11"/>
-      <c r="BH42" s="11"/>
-      <c r="BI42" s="11"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
+      <c r="AD42" s="15"/>
+      <c r="AE42" s="15"/>
+      <c r="AF42" s="15"/>
+      <c r="AG42" s="15"/>
+      <c r="AH42" s="15"/>
+      <c r="AI42" s="15"/>
+      <c r="AJ42" s="15"/>
+      <c r="AK42" s="15"/>
+      <c r="AL42" s="15"/>
+      <c r="AM42" s="15"/>
+      <c r="AN42" s="15"/>
+      <c r="AO42" s="15"/>
+      <c r="AP42" s="15"/>
+      <c r="AQ42" s="15"/>
+      <c r="AR42" s="15"/>
+      <c r="AS42" s="15"/>
+      <c r="AT42" s="15"/>
+      <c r="AU42" s="15"/>
+      <c r="AV42" s="15"/>
+      <c r="AW42" s="15"/>
+      <c r="AX42" s="15"/>
+      <c r="AY42" s="15"/>
+      <c r="AZ42" s="15"/>
+      <c r="BA42" s="15"/>
+      <c r="BB42" s="15"/>
+      <c r="BC42" s="15"/>
+      <c r="BD42" s="15"/>
+      <c r="BE42" s="15"/>
+      <c r="BF42" s="15"/>
+      <c r="BG42" s="15"/>
+      <c r="BH42" s="15"/>
+      <c r="BI42" s="15"/>
       <c r="BJ42" s="11">
         <v>0.5</v>
       </c>
-      <c r="BK42" s="2"/>
+      <c r="BK42" s="9">
+        <v>0.5</v>
+      </c>
       <c r="BL42" s="2"/>
       <c r="BM42" s="2"/>
       <c r="BN42" s="2"/>
@@ -7324,10 +7331,10 @@
       <c r="BP53" s="3"/>
     </row>
     <row r="54" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="30"/>
+      <c r="C54" s="31"/>
       <c r="D54" s="23">
         <f>SUM(D6:D53)</f>
         <v>64</v>
@@ -7458,7 +7465,7 @@
       </c>
       <c r="AJ54" s="5">
         <f t="shared" ref="AJ54" si="14">AI54-SUM(AJ6:AJ53)</f>
-        <v>56</v>
+        <v>56.5</v>
       </c>
       <c r="AK54" s="5">
         <f t="shared" ref="AK54" si="15">AJ54-SUM(AK6:AK53)</f>
@@ -7526,35 +7533,35 @@
       </c>
       <c r="BA54" s="5">
         <f t="shared" ref="BA54" si="29">AZ54-SUM(BA6:BA53)</f>
-        <v>27</v>
+        <v>26.9</v>
       </c>
       <c r="BB54" s="5">
         <f t="shared" ref="BB54" si="30">BA54-SUM(BB6:BB53)</f>
-        <v>27.5</v>
+        <v>27.099999999999998</v>
       </c>
       <c r="BC54" s="5">
         <f t="shared" ref="BC54" si="31">BB54-SUM(BC6:BC53)</f>
-        <v>27.5</v>
+        <v>27.099999999999998</v>
       </c>
       <c r="BD54" s="5">
         <f t="shared" ref="BD54" si="32">BC54-SUM(BD6:BD53)</f>
-        <v>27.5</v>
+        <v>27.099999999999998</v>
       </c>
       <c r="BE54" s="5">
         <f t="shared" ref="BE54" si="33">BD54-SUM(BE6:BE53)</f>
-        <v>27.5</v>
+        <v>27.099999999999998</v>
       </c>
       <c r="BF54" s="5">
         <f t="shared" ref="BF54" si="34">BE54-SUM(BF6:BF53)</f>
-        <v>27.5</v>
+        <v>27.099999999999998</v>
       </c>
       <c r="BG54" s="5">
         <f t="shared" ref="BG54" si="35">BF54-SUM(BG6:BG53)</f>
-        <v>27.5</v>
+        <v>27.099999999999998</v>
       </c>
       <c r="BH54" s="5">
         <f t="shared" ref="BH54" si="36">BG54-SUM(BH6:BH53)</f>
-        <v>27</v>
+        <v>26.9</v>
       </c>
       <c r="BI54" s="5">
         <f t="shared" ref="BI54" si="37">BH54-SUM(BI6:BI53)</f>
@@ -7566,34 +7573,34 @@
       </c>
       <c r="BK54" s="5">
         <f t="shared" si="38"/>
-        <v>17</v>
+        <v>14.5</v>
       </c>
       <c r="BL54" s="5">
         <f t="shared" si="38"/>
-        <v>17</v>
+        <v>14.4</v>
       </c>
       <c r="BM54" s="5">
         <f t="shared" ref="BM54" si="39">BL54-SUM(BM6:BM53)</f>
-        <v>17</v>
+        <v>14.4</v>
       </c>
       <c r="BN54" s="5">
         <f t="shared" ref="BN54" si="40">BM54-SUM(BN6:BN53)</f>
-        <v>17</v>
+        <v>14.4</v>
       </c>
       <c r="BO54" s="5">
         <f t="shared" ref="BO54" si="41">BN54-SUM(BO6:BO53)</f>
-        <v>17</v>
+        <v>14.4</v>
       </c>
       <c r="BP54" s="5">
         <f>BO54-SUM(BP6:BP53)</f>
-        <v>17</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="32"/>
+      <c r="C55" s="33"/>
       <c r="D55" s="6">
         <f>SUM(D6:D53)</f>
         <v>64</v>

</xml_diff>

<commit_message>
pincode functie create, delete, login klaar. index, logout fixed
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4589C53E-86EF-413A-AC0F-933CAEE511AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29FC892-702F-473B-8C1C-7D179BCAF27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
@@ -886,8 +886,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF99"/>
       <color rgb="FFCCFFCC"/>
-      <color rgb="FF99FF99"/>
       <color rgb="FF33CC33"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFF0066"/>
@@ -1399,22 +1399,22 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>14.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>14.2</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>14.2</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>14.2</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>14.2</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>14.2</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3033,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BM9" sqref="BM9"/>
+    <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
+      <selection activeCell="BL16" sqref="BL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4241,74 +4241,76 @@
       <c r="B14" s="20">
         <v>9</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>2</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11"/>
-      <c r="AL14" s="11"/>
-      <c r="AM14" s="11"/>
-      <c r="AN14" s="11"/>
-      <c r="AO14" s="11"/>
-      <c r="AP14" s="11"/>
-      <c r="AQ14" s="11"/>
-      <c r="AR14" s="11"/>
-      <c r="AS14" s="11"/>
-      <c r="AT14" s="11"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+      <c r="AN14" s="15"/>
+      <c r="AO14" s="15"/>
+      <c r="AP14" s="15"/>
+      <c r="AQ14" s="15"/>
+      <c r="AR14" s="15"/>
+      <c r="AS14" s="15"/>
+      <c r="AT14" s="15"/>
       <c r="AU14" s="11">
         <v>1</v>
       </c>
-      <c r="AV14" s="11"/>
-      <c r="AW14" s="11"/>
-      <c r="AX14" s="11"/>
-      <c r="AY14" s="2"/>
-      <c r="AZ14" s="2"/>
-      <c r="BA14" s="2"/>
-      <c r="BB14" s="2"/>
-      <c r="BC14" s="2"/>
-      <c r="BD14" s="2"/>
-      <c r="BE14" s="2"/>
-      <c r="BF14" s="2"/>
-      <c r="BG14" s="2"/>
-      <c r="BH14" s="2"/>
-      <c r="BI14" s="2"/>
-      <c r="BJ14" s="2"/>
-      <c r="BK14" s="2"/>
-      <c r="BL14" s="2"/>
+      <c r="AV14" s="15"/>
+      <c r="AW14" s="15"/>
+      <c r="AX14" s="15"/>
+      <c r="AY14" s="15"/>
+      <c r="AZ14" s="15"/>
+      <c r="BA14" s="15"/>
+      <c r="BB14" s="15"/>
+      <c r="BC14" s="15"/>
+      <c r="BD14" s="15"/>
+      <c r="BE14" s="15"/>
+      <c r="BF14" s="15"/>
+      <c r="BG14" s="15"/>
+      <c r="BH14" s="15"/>
+      <c r="BI14" s="15"/>
+      <c r="BJ14" s="15"/>
+      <c r="BK14" s="15"/>
+      <c r="BL14" s="9">
+        <v>1</v>
+      </c>
       <c r="BM14" s="2"/>
       <c r="BN14" s="2"/>
       <c r="BO14" s="2"/>
@@ -4318,74 +4320,76 @@
       <c r="B15" s="20">
         <v>10</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="9">
         <v>2</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="11"/>
-      <c r="AK15" s="11"/>
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="11"/>
-      <c r="AN15" s="11"/>
-      <c r="AO15" s="11"/>
-      <c r="AP15" s="11"/>
-      <c r="AQ15" s="11"/>
-      <c r="AR15" s="11"/>
-      <c r="AS15" s="11"/>
-      <c r="AT15" s="11"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="15"/>
+      <c r="AK15" s="15"/>
+      <c r="AL15" s="15"/>
+      <c r="AM15" s="15"/>
+      <c r="AN15" s="15"/>
+      <c r="AO15" s="15"/>
+      <c r="AP15" s="15"/>
+      <c r="AQ15" s="15"/>
+      <c r="AR15" s="15"/>
+      <c r="AS15" s="15"/>
+      <c r="AT15" s="15"/>
       <c r="AU15" s="11">
         <v>1</v>
       </c>
-      <c r="AV15" s="11"/>
-      <c r="AW15" s="11"/>
-      <c r="AX15" s="11"/>
-      <c r="AY15" s="2"/>
-      <c r="AZ15" s="2"/>
-      <c r="BA15" s="2"/>
-      <c r="BB15" s="2"/>
-      <c r="BC15" s="2"/>
-      <c r="BD15" s="2"/>
-      <c r="BE15" s="2"/>
-      <c r="BF15" s="2"/>
-      <c r="BG15" s="2"/>
-      <c r="BH15" s="2"/>
-      <c r="BI15" s="2"/>
-      <c r="BJ15" s="2"/>
-      <c r="BK15" s="2"/>
-      <c r="BL15" s="2"/>
+      <c r="AV15" s="15"/>
+      <c r="AW15" s="15"/>
+      <c r="AX15" s="15"/>
+      <c r="AY15" s="15"/>
+      <c r="AZ15" s="15"/>
+      <c r="BA15" s="15"/>
+      <c r="BB15" s="15"/>
+      <c r="BC15" s="15"/>
+      <c r="BD15" s="15"/>
+      <c r="BE15" s="15"/>
+      <c r="BF15" s="15"/>
+      <c r="BG15" s="15"/>
+      <c r="BH15" s="15"/>
+      <c r="BI15" s="15"/>
+      <c r="BJ15" s="15"/>
+      <c r="BK15" s="15"/>
+      <c r="BL15" s="9">
+        <v>1</v>
+      </c>
       <c r="BM15" s="2"/>
       <c r="BN15" s="2"/>
       <c r="BO15" s="2"/>
@@ -4395,74 +4399,76 @@
       <c r="B16" s="20">
         <v>11</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
-      <c r="AI16" s="11"/>
-      <c r="AJ16" s="11"/>
-      <c r="AK16" s="11"/>
-      <c r="AL16" s="11"/>
-      <c r="AM16" s="11"/>
-      <c r="AN16" s="11"/>
-      <c r="AO16" s="11"/>
-      <c r="AP16" s="11"/>
-      <c r="AQ16" s="11"/>
-      <c r="AR16" s="11"/>
-      <c r="AS16" s="11"/>
-      <c r="AT16" s="11"/>
-      <c r="AU16" s="11"/>
-      <c r="AV16" s="11"/>
-      <c r="AW16" s="11"/>
-      <c r="AX16" s="11"/>
-      <c r="AY16" s="11"/>
-      <c r="AZ16" s="11"/>
-      <c r="BA16" s="11"/>
-      <c r="BB16" s="11"/>
-      <c r="BC16" s="11"/>
-      <c r="BD16" s="11"/>
-      <c r="BE16" s="11"/>
-      <c r="BF16" s="11"/>
-      <c r="BG16" s="11"/>
-      <c r="BH16" s="11"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="15"/>
+      <c r="AO16" s="15"/>
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+      <c r="AS16" s="15"/>
+      <c r="AT16" s="15"/>
+      <c r="AU16" s="15"/>
+      <c r="AV16" s="15"/>
+      <c r="AW16" s="15"/>
+      <c r="AX16" s="15"/>
+      <c r="AY16" s="15"/>
+      <c r="AZ16" s="15"/>
+      <c r="BA16" s="15"/>
+      <c r="BB16" s="15"/>
+      <c r="BC16" s="15"/>
+      <c r="BD16" s="15"/>
+      <c r="BE16" s="15"/>
+      <c r="BF16" s="15"/>
+      <c r="BG16" s="15"/>
+      <c r="BH16" s="15"/>
       <c r="BI16" s="11">
         <v>0.5</v>
       </c>
-      <c r="BJ16" s="2"/>
-      <c r="BK16" s="2"/>
-      <c r="BL16" s="2"/>
+      <c r="BJ16" s="15"/>
+      <c r="BK16" s="15"/>
+      <c r="BL16" s="9">
+        <v>0.5</v>
+      </c>
       <c r="BM16" s="2"/>
       <c r="BN16" s="2"/>
       <c r="BO16" s="2"/>
@@ -4616,17 +4622,21 @@
       <c r="BA18" s="9">
         <v>0.5</v>
       </c>
-      <c r="BB18" s="2"/>
-      <c r="BC18" s="2"/>
-      <c r="BD18" s="2"/>
-      <c r="BE18" s="2"/>
-      <c r="BF18" s="2"/>
-      <c r="BG18" s="2"/>
-      <c r="BH18" s="2"/>
-      <c r="BI18" s="2"/>
-      <c r="BJ18" s="2"/>
-      <c r="BK18" s="2"/>
-      <c r="BL18" s="2"/>
+      <c r="BB18" s="15"/>
+      <c r="BC18" s="15"/>
+      <c r="BD18" s="15"/>
+      <c r="BE18" s="15"/>
+      <c r="BF18" s="15"/>
+      <c r="BG18" s="15"/>
+      <c r="BH18" s="15"/>
+      <c r="BI18" s="15"/>
+      <c r="BJ18" s="15"/>
+      <c r="BK18" s="11">
+        <v>-0.5</v>
+      </c>
+      <c r="BL18" s="9">
+        <v>0.5</v>
+      </c>
       <c r="BM18" s="2"/>
       <c r="BN18" s="2"/>
       <c r="BO18" s="2"/>
@@ -7573,27 +7583,27 @@
       </c>
       <c r="BK54" s="5">
         <f t="shared" si="38"/>
-        <v>14.5</v>
+        <v>15</v>
       </c>
       <c r="BL54" s="5">
         <f t="shared" si="38"/>
-        <v>14.2</v>
+        <v>11.7</v>
       </c>
       <c r="BM54" s="5">
         <f t="shared" ref="BM54" si="39">BL54-SUM(BM6:BM53)</f>
-        <v>14.2</v>
+        <v>11.7</v>
       </c>
       <c r="BN54" s="5">
         <f t="shared" ref="BN54" si="40">BM54-SUM(BN6:BN53)</f>
-        <v>14.2</v>
+        <v>11.7</v>
       </c>
       <c r="BO54" s="5">
         <f t="shared" ref="BO54" si="41">BN54-SUM(BO6:BO53)</f>
-        <v>14.2</v>
+        <v>11.7</v>
       </c>
       <c r="BP54" s="5">
         <f>BO54-SUM(BP6:BP53)</f>
-        <v>14.2</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Homepage edited, extra documentatie
</commit_message>
<xml_diff>
--- a/Documentatie/DK_Sprint_Burndown.xlsx
+++ b/Documentatie/DK_Sprint_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DonkeyTravel\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22046DA-EE82-4F4E-ABCE-52B4816F3B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B652B38-503A-47A0-90ED-9AC9ACAEB243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5E3DFA77-994E-40F7-9D1E-9CF86D7BF357}"/>
   </bookViews>
@@ -453,7 +453,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,24 +493,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,7 +737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -801,9 +783,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -857,12 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -871,10 +845,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF99"/>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FF99FF99"/>
-      <color rgb="FFCCFFCC"/>
       <color rgb="FF33CC33"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFF0066"/>
@@ -1212,67 +1186,67 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>63</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>62</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>62</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>62</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>62</c:v>
+                  <c:v>62.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>62</c:v>
+                  <c:v>62.2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>61</c:v>
+                  <c:v>62.2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>62</c:v>
+                  <c:v>62.2</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>59</c:v>
@@ -1296,25 +1270,25 @@
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>56.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>56</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>56</c:v>
+                  <c:v>54.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>55</c:v>
+                  <c:v>54.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>50</c:v>
@@ -1323,7 +1297,7 @@
                   <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>47.5</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>47.5</c:v>
@@ -1341,67 +1315,67 @@
                   <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>32.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>32.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>32.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>32.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>33</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>26.9</c:v>
+                  <c:v>27.4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>27.099999999999998</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>27.099999999999998</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>27.099999999999998</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>27.099999999999998</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>27.099999999999998</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>27.099999999999998</c:v>
+                  <c:v>27.599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>26.9</c:v>
+                  <c:v>27.4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>23.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>17</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>15</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>13.7</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.6999999999999993</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>5.6999999999999993</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.6999999999999993</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2.6999999999999993</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3020,8 +2994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAB2589-B7B2-4C33-8704-E55E84A72B35}">
   <dimension ref="B1:BQ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3035,98 +3009,98 @@
   <sheetData>
     <row r="1" spans="2:69" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:69" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="29"/>
-      <c r="AG2" s="29"/>
-      <c r="AH2" s="29"/>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
-      <c r="AO2" s="29"/>
-      <c r="AP2" s="29"/>
-      <c r="AQ2" s="29"/>
-      <c r="AR2" s="29"/>
-      <c r="AS2" s="29"/>
-      <c r="AT2" s="29"/>
-      <c r="AU2" s="29"/>
-      <c r="AV2" s="29"/>
-      <c r="AW2" s="29"/>
-      <c r="AX2" s="29"/>
-      <c r="AY2" s="29"/>
-      <c r="AZ2" s="29"/>
-      <c r="BA2" s="29"/>
-      <c r="BB2" s="29"/>
-      <c r="BC2" s="29"/>
-      <c r="BD2" s="29"/>
-      <c r="BE2" s="29"/>
-      <c r="BF2" s="29"/>
-      <c r="BG2" s="29"/>
-      <c r="BH2" s="29"/>
-      <c r="BI2" s="29"/>
-      <c r="BJ2" s="29"/>
-      <c r="BK2" s="29"/>
-      <c r="BL2" s="29"/>
-      <c r="BM2" s="29"/>
-      <c r="BN2" s="29"/>
-      <c r="BO2" s="29"/>
-      <c r="BP2" s="29"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="28"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="28"/>
+      <c r="AR2" s="28"/>
+      <c r="AS2" s="28"/>
+      <c r="AT2" s="28"/>
+      <c r="AU2" s="28"/>
+      <c r="AV2" s="28"/>
+      <c r="AW2" s="28"/>
+      <c r="AX2" s="28"/>
+      <c r="AY2" s="28"/>
+      <c r="AZ2" s="28"/>
+      <c r="BA2" s="28"/>
+      <c r="BB2" s="28"/>
+      <c r="BC2" s="28"/>
+      <c r="BD2" s="28"/>
+      <c r="BE2" s="28"/>
+      <c r="BF2" s="28"/>
+      <c r="BG2" s="28"/>
+      <c r="BH2" s="28"/>
+      <c r="BI2" s="28"/>
+      <c r="BJ2" s="28"/>
+      <c r="BK2" s="28"/>
+      <c r="BL2" s="28"/>
+      <c r="BM2" s="28"/>
+      <c r="BN2" s="28"/>
+      <c r="BO2" s="28"/>
+      <c r="BP2" s="28"/>
       <c r="BQ2" s="1"/>
     </row>
     <row r="3" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -3176,10 +3150,10 @@
       <c r="BP3" s="3"/>
     </row>
     <row r="4" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -3379,8 +3353,8 @@
       </c>
     </row>
     <row r="5" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="15" t="s">
         <v>4</v>
       </c>
@@ -3579,7 +3553,7 @@
       <c r="BQ5" s="1"/>
     </row>
     <row r="6" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -3588,23 +3562,23 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
@@ -3656,7 +3630,7 @@
       <c r="BP6" s="2"/>
     </row>
     <row r="7" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -3666,29 +3640,31 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="7">
+        <v>0.1</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -3733,7 +3709,7 @@
       <c r="BP7" s="2"/>
     </row>
     <row r="8" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -3743,29 +3719,31 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="7">
+        <v>0.1</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -3810,7 +3788,7 @@
       <c r="BP8" s="2"/>
     </row>
     <row r="9" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -3850,18 +3828,22 @@
       <c r="AG9" s="13"/>
       <c r="AH9" s="13"/>
       <c r="AI9" s="13"/>
-      <c r="AJ9" s="7">
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="7">
         <v>0.5</v>
       </c>
-      <c r="AK9" s="9">
+      <c r="AM9" s="9">
         <v>-0.5</v>
       </c>
-      <c r="AL9" s="13"/>
-      <c r="AM9" s="13"/>
       <c r="AN9" s="13"/>
       <c r="AO9" s="13"/>
-      <c r="AP9" s="13"/>
-      <c r="AQ9" s="13"/>
+      <c r="AP9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AQ9" s="9">
+        <v>-0.5</v>
+      </c>
       <c r="AR9" s="13"/>
       <c r="AS9" s="13"/>
       <c r="AT9" s="13"/>
@@ -3891,7 +3873,7 @@
       <c r="BJ9" s="13"/>
       <c r="BK9" s="13"/>
       <c r="BL9" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="BM9" s="2"/>
       <c r="BN9" s="2"/>
@@ -3899,7 +3881,7 @@
       <c r="BP9" s="2"/>
     </row>
     <row r="10" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -3941,12 +3923,20 @@
       <c r="AI10" s="13"/>
       <c r="AJ10" s="13"/>
       <c r="AK10" s="13"/>
-      <c r="AL10" s="13"/>
-      <c r="AM10" s="13"/>
+      <c r="AL10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AM10" s="9">
+        <v>-0.5</v>
+      </c>
       <c r="AN10" s="13"/>
       <c r="AO10" s="13"/>
-      <c r="AP10" s="13"/>
-      <c r="AQ10" s="13"/>
+      <c r="AP10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AQ10" s="9">
+        <v>-0.5</v>
+      </c>
       <c r="AR10" s="13"/>
       <c r="AS10" s="13"/>
       <c r="AT10" s="13"/>
@@ -3980,7 +3970,7 @@
       <c r="BP10" s="2"/>
     </row>
     <row r="11" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B11" s="18">
+      <c r="B11" s="17">
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -4057,7 +4047,7 @@
       <c r="BP11" s="2"/>
     </row>
     <row r="12" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -4146,7 +4136,7 @@
       <c r="BP12" s="2"/>
     </row>
     <row r="13" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B13" s="18">
+      <c r="B13" s="17">
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -4225,7 +4215,7 @@
       <c r="BP13" s="2"/>
     </row>
     <row r="14" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <v>9</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -4295,9 +4285,7 @@
       <c r="BI14" s="13"/>
       <c r="BJ14" s="13"/>
       <c r="BK14" s="13"/>
-      <c r="BL14" s="7">
-        <v>1</v>
-      </c>
+      <c r="BL14" s="13"/>
       <c r="BM14" s="7">
         <v>1</v>
       </c>
@@ -4306,7 +4294,7 @@
       <c r="BP14" s="2"/>
     </row>
     <row r="15" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B15" s="18">
+      <c r="B15" s="17">
         <v>10</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -4376,9 +4364,7 @@
       <c r="BI15" s="13"/>
       <c r="BJ15" s="13"/>
       <c r="BK15" s="13"/>
-      <c r="BL15" s="7">
-        <v>1</v>
-      </c>
+      <c r="BL15" s="13"/>
       <c r="BM15" s="7">
         <v>1</v>
       </c>
@@ -4387,7 +4373,7 @@
       <c r="BP15" s="2"/>
     </row>
     <row r="16" spans="2:69" x14ac:dyDescent="0.35">
-      <c r="B16" s="18">
+      <c r="B16" s="17">
         <v>11</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -4466,7 +4452,7 @@
       <c r="BP16" s="2"/>
     </row>
     <row r="17" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <v>12</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -4494,12 +4480,8 @@
       <c r="U17" s="13"/>
       <c r="V17" s="13"/>
       <c r="W17" s="13"/>
-      <c r="X17" s="9">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="9">
-        <v>-1</v>
-      </c>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
       <c r="Z17" s="9">
         <v>1</v>
       </c>
@@ -4549,7 +4531,7 @@
       <c r="BP17" s="2"/>
     </row>
     <row r="18" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B18" s="18">
+      <c r="B18" s="17">
         <v>13</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -4634,7 +4616,7 @@
       <c r="BP18" s="2"/>
     </row>
     <row r="19" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B19" s="18">
+      <c r="B19" s="17">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -4698,7 +4680,6 @@
       <c r="AY19" s="2"/>
       <c r="AZ19" s="2"/>
       <c r="BA19" s="2"/>
-      <c r="BB19" s="2"/>
       <c r="BC19" s="2"/>
       <c r="BD19" s="2"/>
       <c r="BE19" s="2"/>
@@ -4715,7 +4696,7 @@
       <c r="BP19" s="2"/>
     </row>
     <row r="20" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B20" s="18">
+      <c r="B20" s="17">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -4768,7 +4749,7 @@
       <c r="AT20" s="13"/>
       <c r="AU20" s="13"/>
       <c r="AV20" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW20" s="2"/>
       <c r="AX20" s="2"/>
@@ -4792,7 +4773,7 @@
       <c r="BP20" s="2"/>
     </row>
     <row r="21" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -4869,7 +4850,7 @@
       <c r="BP21" s="2"/>
     </row>
     <row r="22" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B22" s="18">
+      <c r="B22" s="17">
         <v>17</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -4946,161 +4927,165 @@
       <c r="BP22" s="2"/>
     </row>
     <row r="23" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B23" s="18">
+      <c r="B23" s="17">
         <v>18</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="7">
         <v>2</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="37"/>
-      <c r="S23" s="37"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="37"/>
-      <c r="Y23" s="37"/>
-      <c r="Z23" s="37"/>
-      <c r="AA23" s="37"/>
-      <c r="AB23" s="37"/>
-      <c r="AC23" s="37"/>
-      <c r="AD23" s="37"/>
-      <c r="AE23" s="37"/>
-      <c r="AF23" s="37"/>
-      <c r="AG23" s="37"/>
-      <c r="AH23" s="37"/>
-      <c r="AI23" s="37"/>
-      <c r="AJ23" s="37"/>
-      <c r="AK23" s="37"/>
-      <c r="AL23" s="37"/>
-      <c r="AM23" s="37"/>
-      <c r="AN23" s="37"/>
-      <c r="AO23" s="37"/>
-      <c r="AP23" s="37"/>
-      <c r="AQ23" s="37"/>
-      <c r="AR23" s="37"/>
-      <c r="AS23" s="37"/>
-      <c r="AT23" s="37"/>
-      <c r="AU23" s="37"/>
-      <c r="AV23" s="37"/>
-      <c r="AW23" s="37"/>
-      <c r="AX23" s="37"/>
-      <c r="AY23" s="37"/>
-      <c r="AZ23" s="37"/>
-      <c r="BA23" s="37"/>
-      <c r="BB23" s="37"/>
-      <c r="BC23" s="37"/>
-      <c r="BD23" s="37"/>
-      <c r="BE23" s="37"/>
-      <c r="BF23" s="37"/>
-      <c r="BG23" s="37"/>
-      <c r="BH23" s="37"/>
-      <c r="BI23" s="37"/>
-      <c r="BJ23" s="37"/>
-      <c r="BK23" s="37"/>
-      <c r="BL23" s="37"/>
-      <c r="BM23" s="37"/>
-      <c r="BN23" s="37"/>
-      <c r="BO23" s="37"/>
-      <c r="BP23" s="37"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="13"/>
+      <c r="AD23" s="13"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="13"/>
+      <c r="AH23" s="13"/>
+      <c r="AI23" s="13"/>
+      <c r="AJ23" s="13"/>
+      <c r="AK23" s="13"/>
+      <c r="AL23" s="13"/>
+      <c r="AM23" s="13"/>
+      <c r="AN23" s="13"/>
+      <c r="AO23" s="13"/>
+      <c r="AP23" s="13"/>
+      <c r="AQ23" s="13"/>
+      <c r="AR23" s="13"/>
+      <c r="AS23" s="13"/>
+      <c r="AT23" s="13"/>
+      <c r="AU23" s="13"/>
+      <c r="AV23" s="13"/>
+      <c r="AW23" s="13"/>
+      <c r="AX23" s="13"/>
+      <c r="AY23" s="13"/>
+      <c r="AZ23" s="13"/>
+      <c r="BA23" s="13"/>
+      <c r="BB23" s="13"/>
+      <c r="BC23" s="13"/>
+      <c r="BD23" s="13"/>
+      <c r="BE23" s="13"/>
+      <c r="BF23" s="13"/>
+      <c r="BG23" s="13"/>
+      <c r="BH23" s="13"/>
+      <c r="BI23" s="13"/>
+      <c r="BJ23" s="13"/>
+      <c r="BK23" s="13"/>
+      <c r="BL23" s="13"/>
+      <c r="BM23" s="13"/>
+      <c r="BN23" s="13"/>
+      <c r="BO23" s="13"/>
+      <c r="BP23" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B24" s="18">
+      <c r="B24" s="17">
         <v>19</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="7">
         <v>2</v>
       </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="37"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="37"/>
-      <c r="Y24" s="37"/>
-      <c r="Z24" s="37"/>
-      <c r="AA24" s="37"/>
-      <c r="AB24" s="37"/>
-      <c r="AC24" s="37"/>
-      <c r="AD24" s="37"/>
-      <c r="AE24" s="37"/>
-      <c r="AF24" s="37"/>
-      <c r="AG24" s="37"/>
-      <c r="AH24" s="37"/>
-      <c r="AI24" s="37"/>
-      <c r="AJ24" s="37"/>
-      <c r="AK24" s="37"/>
-      <c r="AL24" s="37"/>
-      <c r="AM24" s="37"/>
-      <c r="AN24" s="37"/>
-      <c r="AO24" s="37"/>
-      <c r="AP24" s="37"/>
-      <c r="AQ24" s="37"/>
-      <c r="AR24" s="37"/>
-      <c r="AS24" s="37"/>
-      <c r="AT24" s="37"/>
-      <c r="AU24" s="37"/>
-      <c r="AV24" s="37"/>
-      <c r="AW24" s="37"/>
-      <c r="AX24" s="37"/>
-      <c r="AY24" s="37"/>
-      <c r="AZ24" s="37"/>
-      <c r="BA24" s="37"/>
-      <c r="BB24" s="37"/>
-      <c r="BC24" s="37"/>
-      <c r="BD24" s="37"/>
-      <c r="BE24" s="37"/>
-      <c r="BF24" s="37"/>
-      <c r="BG24" s="37"/>
-      <c r="BH24" s="37"/>
-      <c r="BI24" s="37"/>
-      <c r="BJ24" s="37"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
+      <c r="AF24" s="13"/>
+      <c r="AG24" s="13"/>
+      <c r="AH24" s="13"/>
+      <c r="AI24" s="13"/>
+      <c r="AJ24" s="13"/>
+      <c r="AK24" s="13"/>
+      <c r="AL24" s="13"/>
+      <c r="AM24" s="13"/>
+      <c r="AN24" s="13"/>
+      <c r="AO24" s="13"/>
+      <c r="AP24" s="13"/>
+      <c r="AQ24" s="13"/>
+      <c r="AR24" s="13"/>
+      <c r="AS24" s="13"/>
+      <c r="AT24" s="13"/>
+      <c r="AU24" s="13"/>
+      <c r="AV24" s="13"/>
+      <c r="AW24" s="13"/>
+      <c r="AX24" s="13"/>
+      <c r="AY24" s="13"/>
+      <c r="AZ24" s="13"/>
+      <c r="BA24" s="13"/>
+      <c r="BB24" s="13"/>
+      <c r="BC24" s="13"/>
+      <c r="BD24" s="13"/>
+      <c r="BE24" s="13"/>
+      <c r="BF24" s="13"/>
+      <c r="BG24" s="13"/>
+      <c r="BH24" s="13"/>
+      <c r="BI24" s="13"/>
+      <c r="BJ24" s="13"/>
       <c r="BK24" s="7">
         <v>2</v>
       </c>
-      <c r="BL24" s="37">
+      <c r="BL24" s="9">
         <v>-2</v>
       </c>
-      <c r="BM24" s="37"/>
-      <c r="BN24" s="37"/>
-      <c r="BO24" s="37"/>
-      <c r="BP24" s="37"/>
+      <c r="BM24" s="13"/>
+      <c r="BN24" s="13"/>
+      <c r="BO24" s="13"/>
+      <c r="BP24" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B25" s="18">
+      <c r="B25" s="17">
         <v>20</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -5177,7 +5162,7 @@
       <c r="BP25" s="2"/>
     </row>
     <row r="26" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B26" s="18">
+      <c r="B26" s="17">
         <v>21</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -5216,12 +5201,12 @@
       </c>
       <c r="AE26" s="13"/>
       <c r="AF26" s="13"/>
-      <c r="AG26" s="7">
+      <c r="AG26" s="13"/>
+      <c r="AH26" s="13"/>
+      <c r="AI26" s="13"/>
+      <c r="AJ26" s="7">
         <v>1</v>
       </c>
-      <c r="AH26" s="2"/>
-      <c r="AI26" s="2"/>
-      <c r="AJ26" s="2"/>
       <c r="AK26" s="2"/>
       <c r="AL26" s="2"/>
       <c r="AM26" s="2"/>
@@ -5256,7 +5241,7 @@
       <c r="BP26" s="2"/>
     </row>
     <row r="27" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B27" s="18">
+      <c r="B27" s="17">
         <v>22</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -5333,7 +5318,7 @@
       <c r="BP27" s="2"/>
     </row>
     <row r="28" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B28" s="18">
+      <c r="B28" s="17">
         <v>23</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -5410,7 +5395,7 @@
       <c r="BP28" s="2"/>
     </row>
     <row r="29" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B29" s="18">
+      <c r="B29" s="17">
         <v>24</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -5489,7 +5474,7 @@
       <c r="BP29" s="2"/>
     </row>
     <row r="30" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B30" s="18">
+      <c r="B30" s="17">
         <v>25</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -5568,7 +5553,7 @@
       <c r="BP30" s="2"/>
     </row>
     <row r="31" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B31" s="18">
+      <c r="B31" s="17">
         <v>26</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -5645,7 +5630,7 @@
       <c r="BP31" s="2"/>
     </row>
     <row r="32" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B32" s="18">
+      <c r="B32" s="17">
         <v>27</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -5722,7 +5707,7 @@
       <c r="BP32" s="2"/>
     </row>
     <row r="33" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B33" s="18">
+      <c r="B33" s="17">
         <v>28</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -5799,7 +5784,7 @@
       <c r="BP33" s="2"/>
     </row>
     <row r="34" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B34" s="18">
+      <c r="B34" s="17">
         <v>29</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -5876,7 +5861,7 @@
       <c r="BP34" s="2"/>
     </row>
     <row r="35" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B35" s="18">
+      <c r="B35" s="17">
         <v>30</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -5957,7 +5942,7 @@
       <c r="BP35" s="2"/>
     </row>
     <row r="36" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B36" s="18">
+      <c r="B36" s="17">
         <v>31</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -6034,7 +6019,7 @@
       <c r="BP36" s="2"/>
     </row>
     <row r="37" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B37" s="19">
+      <c r="B37" s="18">
         <v>32</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -6111,7 +6096,7 @@
       <c r="BP37" s="4"/>
     </row>
     <row r="38" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B38" s="20">
+      <c r="B38" s="19">
         <v>33</v>
       </c>
       <c r="C38" s="8" t="s">
@@ -6188,10 +6173,10 @@
       <c r="BP38" s="4"/>
     </row>
     <row r="39" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B39" s="19">
+      <c r="B39" s="18">
         <v>34</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="22" t="s">
         <v>112</v>
       </c>
       <c r="D39" s="7">
@@ -6265,10 +6250,10 @@
       <c r="BP39" s="2"/>
     </row>
     <row r="40" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B40" s="20">
+      <c r="B40" s="19">
         <v>35</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="22" t="s">
         <v>113</v>
       </c>
       <c r="D40" s="7">
@@ -6342,10 +6327,10 @@
       <c r="BP40" s="2"/>
     </row>
     <row r="41" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B41" s="19">
+      <c r="B41" s="18">
         <v>36</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="22" t="s">
         <v>114</v>
       </c>
       <c r="D41" s="7">
@@ -6419,10 +6404,10 @@
       <c r="BP41" s="2"/>
     </row>
     <row r="42" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B42" s="20">
+      <c r="B42" s="19">
         <v>37</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="23" t="s">
         <v>115</v>
       </c>
       <c r="D42" s="8">
@@ -6498,7 +6483,7 @@
       <c r="BP42" s="2"/>
     </row>
     <row r="43" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B43" s="19">
+      <c r="B43" s="18">
         <v>38</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -6575,10 +6560,10 @@
       <c r="BP43" s="2"/>
     </row>
     <row r="44" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B44" s="20">
+      <c r="B44" s="19">
         <v>39</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D44" s="7">
@@ -6656,10 +6641,10 @@
       <c r="BP44" s="2"/>
     </row>
     <row r="45" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B45" s="19">
+      <c r="B45" s="18">
         <v>40</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="22" t="s">
         <v>120</v>
       </c>
       <c r="D45" s="7">
@@ -6733,10 +6718,10 @@
       <c r="BP45" s="2"/>
     </row>
     <row r="46" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B46" s="20">
+      <c r="B46" s="19">
         <v>41</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="22" t="s">
         <v>121</v>
       </c>
       <c r="D46" s="7">
@@ -6810,7 +6795,7 @@
       <c r="BP46" s="2"/>
     </row>
     <row r="47" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B47" s="20">
+      <c r="B47" s="19">
         <v>42</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -6887,7 +6872,7 @@
       <c r="BP47" s="2"/>
     </row>
     <row r="48" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B48" s="19">
+      <c r="B48" s="18">
         <v>43</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -6964,7 +6949,7 @@
       <c r="BP48" s="4"/>
     </row>
     <row r="49" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B49" s="20">
+      <c r="B49" s="19">
         <v>44</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -7041,7 +7026,7 @@
       <c r="BP49" s="2"/>
     </row>
     <row r="50" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B50" s="20">
+      <c r="B50" s="19">
         <v>45</v>
       </c>
       <c r="C50" s="7" t="s">
@@ -7118,7 +7103,7 @@
       <c r="BP50" s="2"/>
     </row>
     <row r="51" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B51" s="19">
+      <c r="B51" s="18">
         <v>46</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -7165,112 +7150,114 @@
       <c r="AL51" s="2"/>
       <c r="AM51" s="2"/>
       <c r="AN51" s="2"/>
-      <c r="AO51" s="22"/>
-      <c r="AP51" s="22"/>
-      <c r="AQ51" s="22"/>
-      <c r="AR51" s="22"/>
-      <c r="AS51" s="22"/>
-      <c r="AT51" s="22"/>
-      <c r="AU51" s="22"/>
-      <c r="AV51" s="22"/>
-      <c r="AW51" s="22"/>
-      <c r="AX51" s="22"/>
-      <c r="AY51" s="22"/>
-      <c r="AZ51" s="22"/>
-      <c r="BA51" s="22"/>
-      <c r="BB51" s="22"/>
-      <c r="BC51" s="22"/>
-      <c r="BD51" s="22"/>
-      <c r="BE51" s="22"/>
-      <c r="BF51" s="22"/>
-      <c r="BG51" s="22"/>
-      <c r="BH51" s="22"/>
-      <c r="BI51" s="22"/>
-      <c r="BJ51" s="22"/>
-      <c r="BK51" s="22"/>
-      <c r="BL51" s="22"/>
-      <c r="BM51" s="22"/>
-      <c r="BN51" s="22"/>
-      <c r="BO51" s="22"/>
-      <c r="BP51" s="22"/>
+      <c r="AO51" s="21"/>
+      <c r="AP51" s="21"/>
+      <c r="AQ51" s="21"/>
+      <c r="AR51" s="21"/>
+      <c r="AS51" s="21"/>
+      <c r="AT51" s="21"/>
+      <c r="AU51" s="21"/>
+      <c r="AV51" s="21"/>
+      <c r="AW51" s="21"/>
+      <c r="AX51" s="21"/>
+      <c r="AY51" s="21"/>
+      <c r="AZ51" s="21"/>
+      <c r="BA51" s="21"/>
+      <c r="BB51" s="21"/>
+      <c r="BC51" s="21"/>
+      <c r="BD51" s="21"/>
+      <c r="BE51" s="21"/>
+      <c r="BF51" s="21"/>
+      <c r="BG51" s="21"/>
+      <c r="BH51" s="21"/>
+      <c r="BI51" s="21"/>
+      <c r="BJ51" s="21"/>
+      <c r="BK51" s="21"/>
+      <c r="BL51" s="21"/>
+      <c r="BM51" s="21"/>
+      <c r="BN51" s="21"/>
+      <c r="BO51" s="21"/>
+      <c r="BP51" s="21"/>
     </row>
     <row r="52" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B52" s="20">
+      <c r="B52" s="19">
         <v>47</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="7">
         <v>1</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="2"/>
-      <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
-      <c r="W52" s="2"/>
-      <c r="X52" s="2"/>
-      <c r="Y52" s="2"/>
-      <c r="Z52" s="2"/>
-      <c r="AA52" s="2"/>
-      <c r="AB52" s="2"/>
-      <c r="AC52" s="2"/>
-      <c r="AD52" s="2"/>
-      <c r="AE52" s="2"/>
-      <c r="AF52" s="2"/>
-      <c r="AG52" s="2"/>
-      <c r="AH52" s="2"/>
-      <c r="AI52" s="2"/>
-      <c r="AJ52" s="2"/>
-      <c r="AK52" s="2"/>
-      <c r="AL52" s="2"/>
-      <c r="AM52" s="2"/>
-      <c r="AN52" s="2"/>
-      <c r="AO52" s="3"/>
-      <c r="AP52" s="3"/>
-      <c r="AQ52" s="3"/>
-      <c r="AR52" s="3"/>
-      <c r="AS52" s="3"/>
-      <c r="AT52" s="3"/>
-      <c r="AU52" s="3"/>
-      <c r="AV52" s="3"/>
-      <c r="AW52" s="3"/>
-      <c r="AX52" s="3"/>
-      <c r="AY52" s="3"/>
-      <c r="AZ52" s="3"/>
-      <c r="BA52" s="3"/>
-      <c r="BB52" s="3"/>
-      <c r="BC52" s="3"/>
-      <c r="BD52" s="3"/>
-      <c r="BE52" s="3"/>
-      <c r="BF52" s="3"/>
-      <c r="BG52" s="3"/>
-      <c r="BH52" s="3"/>
-      <c r="BI52" s="3"/>
-      <c r="BJ52" s="3"/>
-      <c r="BK52" s="3"/>
-      <c r="BL52" s="3"/>
-      <c r="BM52" s="3"/>
-      <c r="BN52" s="3"/>
-      <c r="BO52" s="3"/>
-      <c r="BP52" s="3"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="36"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="36"/>
+      <c r="P52" s="36"/>
+      <c r="Q52" s="36"/>
+      <c r="R52" s="36"/>
+      <c r="S52" s="36"/>
+      <c r="T52" s="36"/>
+      <c r="U52" s="36"/>
+      <c r="V52" s="36"/>
+      <c r="W52" s="36"/>
+      <c r="X52" s="36"/>
+      <c r="Y52" s="36"/>
+      <c r="Z52" s="36"/>
+      <c r="AA52" s="36"/>
+      <c r="AB52" s="36"/>
+      <c r="AC52" s="36"/>
+      <c r="AD52" s="36"/>
+      <c r="AE52" s="36"/>
+      <c r="AF52" s="36"/>
+      <c r="AG52" s="36"/>
+      <c r="AH52" s="36"/>
+      <c r="AI52" s="36"/>
+      <c r="AJ52" s="36"/>
+      <c r="AK52" s="36"/>
+      <c r="AL52" s="36"/>
+      <c r="AM52" s="36"/>
+      <c r="AN52" s="36"/>
+      <c r="AO52" s="36"/>
+      <c r="AP52" s="36"/>
+      <c r="AQ52" s="36"/>
+      <c r="AR52" s="36"/>
+      <c r="AS52" s="36"/>
+      <c r="AT52" s="36"/>
+      <c r="AU52" s="36"/>
+      <c r="AV52" s="36"/>
+      <c r="AW52" s="36"/>
+      <c r="AX52" s="36"/>
+      <c r="AY52" s="36"/>
+      <c r="AZ52" s="36"/>
+      <c r="BA52" s="36"/>
+      <c r="BB52" s="36"/>
+      <c r="BC52" s="36"/>
+      <c r="BD52" s="36"/>
+      <c r="BE52" s="36"/>
+      <c r="BF52" s="36"/>
+      <c r="BG52" s="36"/>
+      <c r="BH52" s="36"/>
+      <c r="BI52" s="36"/>
+      <c r="BJ52" s="36"/>
+      <c r="BK52" s="36"/>
+      <c r="BL52" s="36"/>
+      <c r="BM52" s="36"/>
+      <c r="BN52" s="36"/>
+      <c r="BO52" s="36"/>
+      <c r="BP52" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="53" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="20">
+      <c r="B53" s="19">
         <v>48</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -7310,12 +7297,14 @@
       <c r="AG53" s="13"/>
       <c r="AH53" s="13"/>
       <c r="AI53" s="13"/>
-      <c r="AJ53" s="13"/>
-      <c r="AK53" s="13"/>
-      <c r="AL53" s="13"/>
-      <c r="AM53" s="13"/>
+      <c r="AJ53" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AK53" s="36"/>
+      <c r="AL53" s="36"/>
+      <c r="AM53" s="36"/>
       <c r="AN53" s="7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AO53" s="3"/>
       <c r="AP53" s="3"/>
@@ -7347,156 +7336,156 @@
       <c r="BP53" s="3"/>
     </row>
     <row r="54" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C54" s="26"/>
-      <c r="D54" s="21">
+      <c r="C54" s="25"/>
+      <c r="D54" s="20">
         <f>SUM(D6:D53)</f>
         <v>64</v>
       </c>
       <c r="E54" s="5">
         <f>D54-SUM(E6:E53)</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F54" s="5">
         <f>E54-SUM(F6:F53)</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G54" s="5">
         <f t="shared" ref="G54:R54" si="0">F54-SUM(G6:G53)</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H54" s="5">
         <f>G54-SUM(H6:H53)</f>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="O54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="P54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R54" s="5">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="S54" s="5">
         <f t="shared" ref="S54" si="1">R54-SUM(S6:S53)</f>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T54" s="5">
-        <f t="shared" ref="T54" si="2">S54-SUM(T6:T53)</f>
-        <v>62</v>
+        <f>S54-SUM(T6:T53)</f>
+        <v>63</v>
       </c>
       <c r="U54" s="5">
-        <f t="shared" ref="U54" si="3">T54-SUM(U6:U53)</f>
-        <v>62</v>
+        <f t="shared" ref="U54" si="2">T54-SUM(U6:U53)</f>
+        <v>63</v>
       </c>
       <c r="V54" s="5">
-        <f t="shared" ref="V54" si="4">U54-SUM(V6:V53)</f>
-        <v>62</v>
+        <f t="shared" ref="V54" si="3">U54-SUM(V6:V53)</f>
+        <v>62.2</v>
       </c>
       <c r="W54" s="5">
-        <f t="shared" ref="W54" si="5">V54-SUM(W6:W53)</f>
-        <v>62</v>
+        <f t="shared" ref="W54" si="4">V54-SUM(W6:W53)</f>
+        <v>62.2</v>
       </c>
       <c r="X54" s="5">
-        <f t="shared" ref="X54" si="6">W54-SUM(X6:X53)</f>
-        <v>61</v>
+        <f t="shared" ref="X54" si="5">W54-SUM(X6:X53)</f>
+        <v>62.2</v>
       </c>
       <c r="Y54" s="5">
-        <f t="shared" ref="Y54" si="7">X54-SUM(Y6:Y53)</f>
-        <v>62</v>
+        <f t="shared" ref="Y54" si="6">X54-SUM(Y6:Y53)</f>
+        <v>62.2</v>
       </c>
       <c r="Z54" s="5">
-        <f t="shared" ref="Z54" si="8">Y54-SUM(Z6:Z53)</f>
+        <f t="shared" ref="Z54" si="7">Y54-SUM(Z6:Z53)</f>
         <v>59</v>
       </c>
       <c r="AA54" s="5">
-        <f t="shared" ref="AA54" si="9">Z54-SUM(AA6:AA53)</f>
+        <f t="shared" ref="AA54" si="8">Z54-SUM(AA6:AA53)</f>
         <v>60</v>
       </c>
       <c r="AB54" s="5">
-        <f t="shared" ref="AB54:AD54" si="10">AA54-SUM(AB6:AB53)</f>
+        <f t="shared" ref="AB54:AD54" si="9">AA54-SUM(AB6:AB53)</f>
         <v>60</v>
       </c>
       <c r="AC54" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="AD54" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>59</v>
       </c>
       <c r="AE54" s="5">
-        <f t="shared" ref="AE54" si="11">AD54-SUM(AE6:AE53)</f>
+        <f t="shared" ref="AE54" si="10">AD54-SUM(AE6:AE53)</f>
         <v>59</v>
       </c>
       <c r="AF54" s="5">
-        <f t="shared" ref="AF54" si="12">AE54-SUM(AF6:AF53)</f>
+        <f t="shared" ref="AF54" si="11">AE54-SUM(AF6:AF53)</f>
         <v>59</v>
       </c>
       <c r="AG54" s="5">
-        <f t="shared" ref="AG54:AI54" si="13">AF54-SUM(AG6:AG53)</f>
-        <v>58</v>
+        <f t="shared" ref="AG54:AI54" si="12">AF54-SUM(AG6:AG53)</f>
+        <v>59</v>
       </c>
       <c r="AH54" s="5">
-        <f t="shared" si="13"/>
-        <v>58</v>
+        <f t="shared" si="12"/>
+        <v>59</v>
       </c>
       <c r="AI54" s="5">
-        <f t="shared" si="13"/>
-        <v>58</v>
+        <f t="shared" si="12"/>
+        <v>59</v>
       </c>
       <c r="AJ54" s="5">
-        <f t="shared" ref="AJ54" si="14">AI54-SUM(AJ6:AJ53)</f>
+        <f t="shared" ref="AJ54" si="13">AI54-SUM(AJ6:AJ53)</f>
         <v>56.5</v>
       </c>
       <c r="AK54" s="5">
-        <f t="shared" ref="AK54" si="15">AJ54-SUM(AK6:AK53)</f>
-        <v>56</v>
+        <f t="shared" ref="AK54" si="14">AJ54-SUM(AK6:AK53)</f>
+        <v>55.5</v>
       </c>
       <c r="AL54" s="5">
-        <f t="shared" ref="AL54" si="16">AK54-SUM(AL6:AL53)</f>
-        <v>56</v>
+        <f t="shared" ref="AL54" si="15">AK54-SUM(AL6:AL53)</f>
+        <v>54.5</v>
       </c>
       <c r="AM54" s="5">
         <f>AL54-SUM(AM6:AM53)</f>
-        <v>55</v>
+        <v>54.5</v>
       </c>
       <c r="AN54" s="5">
-        <f t="shared" ref="AN54" si="17">AM54-SUM(AN6:AN53)</f>
+        <f t="shared" ref="AN54" si="16">AM54-SUM(AN6:AN53)</f>
         <v>50</v>
       </c>
       <c r="AO54" s="5">
@@ -7504,119 +7493,119 @@
         <v>50.5</v>
       </c>
       <c r="AP54" s="5">
-        <f t="shared" ref="AP54" si="18">AO54-SUM(AP6:AP53)</f>
+        <f t="shared" ref="AP54" si="17">AO54-SUM(AP6:AP53)</f>
+        <v>46.5</v>
+      </c>
+      <c r="AQ54" s="5">
+        <f t="shared" ref="AQ54" si="18">AP54-SUM(AQ6:AQ53)</f>
         <v>47.5</v>
       </c>
-      <c r="AQ54" s="5">
-        <f t="shared" ref="AQ54" si="19">AP54-SUM(AQ6:AQ53)</f>
-        <v>47.5</v>
-      </c>
       <c r="AR54" s="5">
-        <f t="shared" ref="AR54" si="20">AQ54-SUM(AR6:AR53)</f>
+        <f t="shared" ref="AR54" si="19">AQ54-SUM(AR6:AR53)</f>
         <v>46.5</v>
       </c>
       <c r="AS54" s="5">
-        <f t="shared" ref="AS54" si="21">AR54-SUM(AS6:AS53)</f>
+        <f t="shared" ref="AS54" si="20">AR54-SUM(AS6:AS53)</f>
         <v>42.5</v>
       </c>
       <c r="AT54" s="5">
-        <f t="shared" ref="AT54" si="22">AS54-SUM(AT6:AT53)</f>
+        <f t="shared" ref="AT54" si="21">AS54-SUM(AT6:AT53)</f>
         <v>42.5</v>
       </c>
       <c r="AU54" s="5">
-        <f t="shared" ref="AU54" si="23">AT54-SUM(AU6:AU53)</f>
+        <f t="shared" ref="AU54" si="22">AT54-SUM(AU6:AU53)</f>
         <v>33.5</v>
       </c>
       <c r="AV54" s="5">
-        <f t="shared" ref="AV54" si="24">AU54-SUM(AV6:AV53)</f>
-        <v>32.5</v>
+        <f t="shared" ref="AV54" si="23">AU54-SUM(AV6:AV53)</f>
+        <v>33</v>
       </c>
       <c r="AW54" s="5">
-        <f t="shared" ref="AW54" si="25">AV54-SUM(AW6:AW53)</f>
-        <v>32.5</v>
+        <f t="shared" ref="AW54" si="24">AV54-SUM(AW6:AW53)</f>
+        <v>33</v>
       </c>
       <c r="AX54" s="5">
-        <f t="shared" ref="AX54" si="26">AW54-SUM(AX6:AX53)</f>
-        <v>32.5</v>
+        <f t="shared" ref="AX54" si="25">AW54-SUM(AX6:AX53)</f>
+        <v>33</v>
       </c>
       <c r="AY54" s="5">
-        <f t="shared" ref="AY54" si="27">AX54-SUM(AY6:AY53)</f>
-        <v>32.5</v>
+        <f t="shared" ref="AY54" si="26">AX54-SUM(AY6:AY53)</f>
+        <v>33</v>
       </c>
       <c r="AZ54" s="5">
-        <f t="shared" ref="AZ54" si="28">AY54-SUM(AZ6:AZ53)</f>
-        <v>33</v>
+        <f t="shared" ref="AZ54" si="27">AY54-SUM(AZ6:AZ53)</f>
+        <v>33.5</v>
       </c>
       <c r="BA54" s="5">
-        <f t="shared" ref="BA54" si="29">AZ54-SUM(BA6:BA53)</f>
-        <v>26.9</v>
+        <f t="shared" ref="BA54" si="28">AZ54-SUM(BA6:BA53)</f>
+        <v>27.4</v>
       </c>
       <c r="BB54" s="5">
-        <f t="shared" ref="BB54" si="30">BA54-SUM(BB6:BB53)</f>
-        <v>27.099999999999998</v>
+        <f t="shared" ref="BB54" si="29">BA54-SUM(BB6:BB53)</f>
+        <v>27.599999999999998</v>
       </c>
       <c r="BC54" s="5">
-        <f t="shared" ref="BC54" si="31">BB54-SUM(BC6:BC53)</f>
-        <v>27.099999999999998</v>
+        <f t="shared" ref="BC54" si="30">BB54-SUM(BC6:BC53)</f>
+        <v>27.599999999999998</v>
       </c>
       <c r="BD54" s="5">
-        <f t="shared" ref="BD54" si="32">BC54-SUM(BD6:BD53)</f>
-        <v>27.099999999999998</v>
+        <f t="shared" ref="BD54" si="31">BC54-SUM(BD6:BD53)</f>
+        <v>27.599999999999998</v>
       </c>
       <c r="BE54" s="5">
-        <f t="shared" ref="BE54" si="33">BD54-SUM(BE6:BE53)</f>
-        <v>27.099999999999998</v>
+        <f t="shared" ref="BE54" si="32">BD54-SUM(BE6:BE53)</f>
+        <v>27.599999999999998</v>
       </c>
       <c r="BF54" s="5">
-        <f t="shared" ref="BF54" si="34">BE54-SUM(BF6:BF53)</f>
-        <v>27.099999999999998</v>
+        <f t="shared" ref="BF54" si="33">BE54-SUM(BF6:BF53)</f>
+        <v>27.599999999999998</v>
       </c>
       <c r="BG54" s="5">
-        <f t="shared" ref="BG54" si="35">BF54-SUM(BG6:BG53)</f>
-        <v>27.099999999999998</v>
+        <f t="shared" ref="BG54" si="34">BF54-SUM(BG6:BG53)</f>
+        <v>27.599999999999998</v>
       </c>
       <c r="BH54" s="5">
-        <f t="shared" ref="BH54" si="36">BG54-SUM(BH6:BH53)</f>
-        <v>26.9</v>
+        <f t="shared" ref="BH54" si="35">BG54-SUM(BH6:BH53)</f>
+        <v>27.4</v>
       </c>
       <c r="BI54" s="5">
-        <f t="shared" ref="BI54" si="37">BH54-SUM(BI6:BI53)</f>
-        <v>23.5</v>
+        <f t="shared" ref="BI54" si="36">BH54-SUM(BI6:BI53)</f>
+        <v>24</v>
       </c>
       <c r="BJ54" s="5">
-        <f t="shared" ref="BJ54:BL54" si="38">BI54-SUM(BJ6:BJ53)</f>
-        <v>17</v>
+        <f t="shared" ref="BJ54:BL54" si="37">BI54-SUM(BJ6:BJ53)</f>
+        <v>17.5</v>
       </c>
       <c r="BK54" s="5">
-        <f t="shared" si="38"/>
-        <v>15</v>
+        <f t="shared" si="37"/>
+        <v>15.5</v>
       </c>
       <c r="BL54" s="5">
-        <f t="shared" si="38"/>
-        <v>13.7</v>
+        <f t="shared" si="37"/>
+        <v>16</v>
       </c>
       <c r="BM54" s="5">
-        <f t="shared" ref="BM54" si="39">BL54-SUM(BM6:BM53)</f>
-        <v>5.6999999999999993</v>
+        <f t="shared" ref="BM54" si="38">BL54-SUM(BM6:BM53)</f>
+        <v>8</v>
       </c>
       <c r="BN54" s="5">
-        <f t="shared" ref="BN54" si="40">BM54-SUM(BN6:BN53)</f>
-        <v>5.6999999999999993</v>
+        <f t="shared" ref="BN54" si="39">BM54-SUM(BN6:BN53)</f>
+        <v>8</v>
       </c>
       <c r="BO54" s="5">
-        <f t="shared" ref="BO54" si="41">BN54-SUM(BO6:BO53)</f>
-        <v>2.6999999999999993</v>
+        <f t="shared" ref="BO54" si="40">BN54-SUM(BO6:BO53)</f>
+        <v>5</v>
       </c>
       <c r="BP54" s="5">
         <f>BO54-SUM(BP6:BP53)</f>
-        <v>2.6999999999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:68" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="27" t="s">
+      <c r="B55" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="28"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="6">
         <f>SUM(D6:D53)</f>
         <v>64</v>

</xml_diff>